<commit_message>
Data analysis updates and Paper draft- methods section changed
</commit_message>
<xml_diff>
--- a/Masters Project Data.xlsx
+++ b/Masters Project Data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="454">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1353,6 +1353,39 @@
   <si>
     <t>Significant at 5%</t>
   </si>
+  <si>
+    <t>http://www.jeremymiles.co.uk/usingstatistics/chapter8/sigofrexcel.html</t>
+  </si>
+  <si>
+    <t>% Rates Highly</t>
+  </si>
+  <si>
+    <t>% Rates Lowly</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>ST DEV</t>
+  </si>
+  <si>
+    <t>wysiwyg vs shortdes</t>
+  </si>
+  <si>
+    <t>wysiwyg vs intention</t>
+  </si>
+  <si>
+    <t>wysiwyg vs emotion</t>
+  </si>
+  <si>
+    <t>shortdes vs intention</t>
+  </si>
+  <si>
+    <t>shortdes vs emotion</t>
+  </si>
+  <si>
+    <t>intention vs emotion</t>
+  </si>
 </sst>
 </file>
 
@@ -1540,7 +1573,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="35">
+  <borders count="38">
     <border>
       <left/>
       <right/>
@@ -1942,8 +1975,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="192">
+  <cellStyleXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2136,8 +2206,10 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="170">
+  <cellXfs count="174">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -2416,8 +2488,12 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="24" fillId="5" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="151" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="192">
+  <cellStyles count="194">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2513,6 +2589,7 @@
     <cellStyle name="Followed Hyperlink" xfId="187" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2608,6 +2685,7 @@
     <cellStyle name="Hyperlink" xfId="186" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="151" builtinId="5"/>
   </cellStyles>
@@ -13262,10 +13340,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:FI135"/>
+  <dimension ref="A1:FK135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CQ36" workbookViewId="0">
-      <selection activeCell="EH87" sqref="EH87"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="FL21" sqref="FL21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -13412,10 +13490,12 @@
     <col min="146" max="146" width="9.33203125" style="6" customWidth="1"/>
     <col min="147" max="147" width="21.5" customWidth="1"/>
     <col min="148" max="148" width="13.5" style="6" customWidth="1"/>
-    <col min="149" max="16384" width="14.5" style="6"/>
+    <col min="149" max="166" width="14.5" style="6"/>
+    <col min="167" max="167" width="18" style="6" customWidth="1"/>
+    <col min="168" max="16384" width="14.5" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:165" ht="23" customHeight="1">
+    <row r="1" spans="1:167" ht="23" customHeight="1">
       <c r="A1" s="16"/>
       <c r="B1" s="137" t="s">
         <v>233</v>
@@ -13565,7 +13645,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:165" ht="21" customHeight="1">
+    <row r="2" spans="1:167" ht="21" customHeight="1">
       <c r="A2" s="16"/>
       <c r="B2" s="137"/>
       <c r="C2" s="10"/>
@@ -13774,7 +13854,7 @@
       <c r="EP2" s="102"/>
       <c r="FD2" s="141"/>
     </row>
-    <row r="3" spans="1:165" ht="17" customHeight="1">
+    <row r="3" spans="1:167" ht="17" customHeight="1">
       <c r="A3" s="16"/>
       <c r="B3" s="137"/>
       <c r="C3" s="10"/>
@@ -14226,7 +14306,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="4" spans="1:165" ht="15.75" customHeight="1">
+    <row r="4" spans="1:167" ht="15.75" customHeight="1">
       <c r="A4" s="7"/>
       <c r="B4" s="8">
         <v>1</v>
@@ -14758,7 +14838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:165" ht="15.75" customHeight="1">
+    <row r="5" spans="1:167" ht="15.75" customHeight="1">
       <c r="A5" s="7"/>
       <c r="B5" s="8">
         <v>1</v>
@@ -15290,7 +15370,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:165" ht="15.75" customHeight="1">
+    <row r="6" spans="1:167" ht="15.75" customHeight="1">
       <c r="A6" s="7"/>
       <c r="B6" s="8">
         <v>2</v>
@@ -15822,7 +15902,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:165" ht="15.75" customHeight="1">
+    <row r="7" spans="1:167" ht="15.75" customHeight="1">
       <c r="A7" s="7"/>
       <c r="B7" s="8">
         <v>2</v>
@@ -16355,7 +16435,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:165" ht="15.75" customHeight="1">
+    <row r="8" spans="1:167" ht="15.75" customHeight="1">
       <c r="A8" s="7"/>
       <c r="B8" s="8">
         <v>2</v>
@@ -16886,8 +16966,11 @@
       <c r="FI8" s="3">
         <v>1</v>
       </c>
+      <c r="FK8" s="6" t="s">
+        <v>448</v>
+      </c>
     </row>
-    <row r="9" spans="1:165" ht="15.75" customHeight="1">
+    <row r="9" spans="1:167" ht="15.75" customHeight="1">
       <c r="A9" s="7"/>
       <c r="B9" s="8">
         <v>1</v>
@@ -17418,8 +17501,12 @@
       <c r="FI9" s="3">
         <v>2</v>
       </c>
+      <c r="FK9" s="6">
+        <f>TTEST(FF4:FF47,FG4:FG47,2,1)</f>
+        <v>7.8756895616448871E-2</v>
+      </c>
     </row>
-    <row r="10" spans="1:165" ht="15.75" customHeight="1">
+    <row r="10" spans="1:167" ht="15.75" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" s="8">
         <v>2</v>
@@ -17952,7 +18039,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:165" ht="15.75" customHeight="1">
+    <row r="11" spans="1:167" ht="15.75" customHeight="1">
       <c r="A11" s="7"/>
       <c r="B11" s="8">
         <v>1</v>
@@ -18483,8 +18570,11 @@
       <c r="FI11" s="3">
         <v>4</v>
       </c>
+      <c r="FK11" s="6" t="s">
+        <v>449</v>
+      </c>
     </row>
-    <row r="12" spans="1:165" ht="15.75" customHeight="1">
+    <row r="12" spans="1:167" ht="15.75" customHeight="1">
       <c r="A12" s="7"/>
       <c r="B12" s="8">
         <v>1</v>
@@ -19015,8 +19105,12 @@
       <c r="FI12" s="3">
         <v>2</v>
       </c>
+      <c r="FK12" s="6">
+        <f>TTEST(FF4:FF47,FH4:FH47,2,1)</f>
+        <v>0.320394370157979</v>
+      </c>
     </row>
-    <row r="13" spans="1:165" ht="15.75" customHeight="1">
+    <row r="13" spans="1:167" ht="15.75" customHeight="1">
       <c r="A13" s="7"/>
       <c r="B13" s="8">
         <v>1</v>
@@ -19548,7 +19642,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:165" ht="15.75" customHeight="1">
+    <row r="14" spans="1:167" ht="15.75" customHeight="1">
       <c r="A14" s="7"/>
       <c r="B14" s="8">
         <v>1</v>
@@ -20079,8 +20173,11 @@
       <c r="FI14" s="3">
         <v>1</v>
       </c>
+      <c r="FK14" s="6" t="s">
+        <v>450</v>
+      </c>
     </row>
-    <row r="15" spans="1:165" ht="15.75" customHeight="1">
+    <row r="15" spans="1:167" ht="15.75" customHeight="1">
       <c r="A15" s="7"/>
       <c r="B15" s="8">
         <v>1</v>
@@ -20612,8 +20709,12 @@
       <c r="FI15" s="3">
         <v>1</v>
       </c>
+      <c r="FK15" s="6">
+        <f>TTEST(FF4:FF47,FI4:FI47,2,1)</f>
+        <v>0.10695292470792205</v>
+      </c>
     </row>
-    <row r="16" spans="1:165" ht="15.75" customHeight="1">
+    <row r="16" spans="1:167" ht="15.75" customHeight="1">
       <c r="A16" s="7"/>
       <c r="B16" s="8">
         <v>1</v>
@@ -21145,7 +21246,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:165" ht="15.75" customHeight="1">
+    <row r="17" spans="1:167" ht="15.75" customHeight="1">
       <c r="A17" s="7"/>
       <c r="B17" s="8">
         <v>2</v>
@@ -21676,8 +21777,11 @@
       <c r="FI17" s="3">
         <v>1</v>
       </c>
+      <c r="FK17" s="6" t="s">
+        <v>451</v>
+      </c>
     </row>
-    <row r="18" spans="1:165" ht="15.75" customHeight="1">
+    <row r="18" spans="1:167" ht="15.75" customHeight="1">
       <c r="A18" s="7"/>
       <c r="B18" s="8">
         <v>1</v>
@@ -22209,8 +22313,12 @@
       <c r="FI18" s="3">
         <v>4</v>
       </c>
+      <c r="FK18" s="6">
+        <f>TTEST(FG4:FG47,FH4:FH47,2,1)</f>
+        <v>0.64345522727804283</v>
+      </c>
     </row>
-    <row r="19" spans="1:165" ht="18">
+    <row r="19" spans="1:167" ht="19" thickBot="1">
       <c r="A19" s="7"/>
       <c r="B19" s="8">
         <v>1</v>
@@ -22743,7 +22851,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:165" ht="15.75" customHeight="1">
+    <row r="20" spans="1:167" ht="15.75" customHeight="1">
       <c r="A20" s="7"/>
       <c r="B20" s="8">
         <v>1</v>
@@ -23274,8 +23382,11 @@
       <c r="FI20" s="3">
         <v>3</v>
       </c>
+      <c r="FK20" s="171" t="s">
+        <v>452</v>
+      </c>
     </row>
-    <row r="21" spans="1:165" ht="15.75" customHeight="1">
+    <row r="21" spans="1:167" ht="15.75" customHeight="1">
       <c r="A21" s="7"/>
       <c r="B21" s="8">
         <v>1</v>
@@ -23807,8 +23918,12 @@
       <c r="FI21" s="3">
         <v>1</v>
       </c>
+      <c r="FK21" s="172">
+        <f>TTEST(FG4:FG47,FI4:FI47,2,1)</f>
+        <v>1.82772962096142E-3</v>
+      </c>
     </row>
-    <row r="22" spans="1:165" ht="15.75" customHeight="1">
+    <row r="22" spans="1:167" ht="15.75" customHeight="1">
       <c r="A22" s="7"/>
       <c r="B22" s="8">
         <v>1</v>
@@ -24339,8 +24454,9 @@
       <c r="FI22" s="3">
         <v>2</v>
       </c>
+      <c r="FK22" s="172"/>
     </row>
-    <row r="23" spans="1:165" ht="15.75" customHeight="1">
+    <row r="23" spans="1:167" ht="15.75" customHeight="1">
       <c r="A23" s="7"/>
       <c r="B23" s="8">
         <v>1</v>
@@ -24871,8 +24987,11 @@
       <c r="FI23" s="3">
         <v>2</v>
       </c>
+      <c r="FK23" s="172" t="s">
+        <v>453</v>
+      </c>
     </row>
-    <row r="24" spans="1:165" ht="15.75" customHeight="1">
+    <row r="24" spans="1:167" ht="15.75" customHeight="1" thickBot="1">
       <c r="A24" s="7"/>
       <c r="B24" s="8">
         <v>1</v>
@@ -25403,8 +25522,12 @@
       <c r="FI24" s="3">
         <v>4</v>
       </c>
+      <c r="FK24" s="173">
+        <f>TTEST(FH4:FH47,FI4:FI47,2,1)</f>
+        <v>3.9848349682986814E-4</v>
+      </c>
     </row>
-    <row r="25" spans="1:165" ht="15.75" customHeight="1">
+    <row r="25" spans="1:167" ht="15.75" customHeight="1">
       <c r="A25" s="7"/>
       <c r="B25" s="8">
         <v>1</v>
@@ -25936,7 +26059,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:165" ht="15.75" customHeight="1">
+    <row r="26" spans="1:167" ht="15.75" customHeight="1">
       <c r="A26" s="7"/>
       <c r="B26" s="8">
         <v>1</v>
@@ -26469,7 +26592,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:165" ht="15.75" customHeight="1">
+    <row r="27" spans="1:167" ht="15.75" customHeight="1">
       <c r="A27" s="7"/>
       <c r="B27" s="8">
         <v>1</v>
@@ -27001,7 +27124,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:165" ht="15.75" customHeight="1">
+    <row r="28" spans="1:167" ht="15.75" customHeight="1">
       <c r="A28" s="7"/>
       <c r="B28" s="8">
         <v>1</v>
@@ -27533,7 +27656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:165" ht="15.75" customHeight="1">
+    <row r="29" spans="1:167" ht="15.75" customHeight="1">
       <c r="A29" s="7"/>
       <c r="B29" s="8">
         <v>2</v>
@@ -28065,7 +28188,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:165" ht="15.75" customHeight="1">
+    <row r="30" spans="1:167" ht="15.75" customHeight="1">
       <c r="A30" s="7"/>
       <c r="B30" s="8">
         <v>2</v>
@@ -28597,7 +28720,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:165" ht="15.75" customHeight="1">
+    <row r="31" spans="1:167" ht="15.75" customHeight="1">
       <c r="A31" s="7"/>
       <c r="B31" s="8">
         <v>1</v>
@@ -29129,7 +29252,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:165" ht="15.75" customHeight="1">
+    <row r="32" spans="1:167" ht="15.75" customHeight="1">
       <c r="A32" s="7"/>
       <c r="B32" s="8">
         <v>1</v>
@@ -37689,6 +37812,25 @@
       <c r="DU48" s="13"/>
       <c r="EA48" s="13"/>
       <c r="EB48" s="66"/>
+      <c r="FE48" s="6" t="s">
+        <v>446</v>
+      </c>
+      <c r="FF48" s="93">
+        <f>AVERAGE(FF4:FF47)</f>
+        <v>2.4318181818181817</v>
+      </c>
+      <c r="FG48" s="93">
+        <f t="shared" ref="FG48:FI48" si="58">AVERAGE(FG4:FG47)</f>
+        <v>2.8636363636363638</v>
+      </c>
+      <c r="FH48" s="93">
+        <f t="shared" si="58"/>
+        <v>2.75</v>
+      </c>
+      <c r="FI48" s="93">
+        <f t="shared" si="58"/>
+        <v>1.9545454545454546</v>
+      </c>
     </row>
     <row r="49" spans="1:165" ht="25" customHeight="1" thickBot="1">
       <c r="A49" s="7"/>
@@ -37749,6 +37891,25 @@
       </c>
       <c r="ER49" s="6" t="s">
         <v>409</v>
+      </c>
+      <c r="FE49" s="6" t="s">
+        <v>447</v>
+      </c>
+      <c r="FF49" s="93">
+        <f>_xlfn.STDEV.S(FF4:FF47)</f>
+        <v>1.2275467550935906</v>
+      </c>
+      <c r="FG49" s="93">
+        <f t="shared" ref="FG49:FI49" si="59">_xlfn.STDEV.S(FG4:FG47)</f>
+        <v>0.97863001277436223</v>
+      </c>
+      <c r="FH49" s="93">
+        <f t="shared" si="59"/>
+        <v>1.0371024035016201</v>
+      </c>
+      <c r="FI49" s="93">
+        <f t="shared" si="59"/>
+        <v>1.0332730892438855</v>
       </c>
     </row>
     <row r="50" spans="1:165" ht="20" customHeight="1" thickBot="1">
@@ -37921,47 +38082,47 @@
         <v>35</v>
       </c>
       <c r="EF51" s="6">
-        <f t="shared" ref="EF51:EP51" si="58">COUNTIF(EF4:EF47,1)</f>
+        <f t="shared" ref="EF51:EP51" si="60">COUNTIF(EF4:EF47,1)</f>
         <v>26</v>
       </c>
       <c r="EG51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>16</v>
       </c>
       <c r="EH51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>26</v>
       </c>
       <c r="EI51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>19</v>
       </c>
       <c r="EJ51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>29</v>
       </c>
       <c r="EK51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>24</v>
       </c>
       <c r="EL51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>5</v>
       </c>
       <c r="EM51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>17</v>
       </c>
       <c r="EN51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>14</v>
       </c>
       <c r="EO51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>23</v>
       </c>
       <c r="EP51" s="6">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>13</v>
       </c>
       <c r="ER51" s="6">
@@ -37969,43 +38130,43 @@
         <v>29</v>
       </c>
       <c r="ES51" s="6">
-        <f t="shared" ref="ES51:FB51" si="59">COUNTIF(ES4:ES47,1)</f>
+        <f t="shared" ref="ES51:FB51" si="61">COUNTIF(ES4:ES47,1)</f>
         <v>26</v>
       </c>
       <c r="ET51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>22</v>
       </c>
       <c r="EU51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>27</v>
       </c>
       <c r="EV51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>17</v>
       </c>
       <c r="EW51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>13</v>
       </c>
       <c r="EX51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>13</v>
       </c>
       <c r="EY51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>6</v>
       </c>
       <c r="EZ51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>12</v>
       </c>
       <c r="FA51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>23</v>
       </c>
       <c r="FB51" s="6">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>10</v>
       </c>
       <c r="FC51" s="75" t="s">
@@ -38018,6 +38179,22 @@
       <c r="FE51" s="152">
         <f>FD51/$FD$56</f>
         <v>0.45454545454545453</v>
+      </c>
+      <c r="FF51" s="6">
+        <f>COUNTIF(FF$4:FF$47,4)</f>
+        <v>13</v>
+      </c>
+      <c r="FG51" s="6">
+        <f t="shared" ref="FG51:FI51" si="62">COUNTIF(FG$4:FG$47,4)</f>
+        <v>13</v>
+      </c>
+      <c r="FH51" s="6">
+        <f t="shared" si="62"/>
+        <v>13</v>
+      </c>
+      <c r="FI51" s="6">
+        <f t="shared" si="62"/>
+        <v>5</v>
       </c>
     </row>
     <row r="52" spans="1:165" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
@@ -38090,47 +38267,47 @@
         <v>9</v>
       </c>
       <c r="EF52" s="13">
-        <f t="shared" ref="EF52:EP52" si="60">COUNTIF(EF4:EF47,0)</f>
+        <f t="shared" ref="EF52:EP52" si="63">COUNTIF(EF4:EF47,0)</f>
         <v>18</v>
       </c>
       <c r="EG52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>28</v>
       </c>
       <c r="EH52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>18</v>
       </c>
       <c r="EI52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>25</v>
       </c>
       <c r="EJ52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>15</v>
       </c>
       <c r="EK52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>20</v>
       </c>
       <c r="EL52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>39</v>
       </c>
       <c r="EM52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>27</v>
       </c>
       <c r="EN52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>30</v>
       </c>
       <c r="EO52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>21</v>
       </c>
       <c r="EP52" s="13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="63"/>
         <v>31</v>
       </c>
       <c r="EQ52"/>
@@ -38139,43 +38316,43 @@
         <v>15</v>
       </c>
       <c r="ES52" s="13">
-        <f t="shared" ref="ES52:FB52" si="61">COUNTIF(ES4:ES47,0)</f>
+        <f t="shared" ref="ES52:FB52" si="64">COUNTIF(ES4:ES47,0)</f>
         <v>18</v>
       </c>
       <c r="ET52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>22</v>
       </c>
       <c r="EU52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>17</v>
       </c>
       <c r="EV52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>27</v>
       </c>
       <c r="EW52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>31</v>
       </c>
       <c r="EX52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>31</v>
       </c>
       <c r="EY52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>38</v>
       </c>
       <c r="EZ52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>32</v>
       </c>
       <c r="FA52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>21</v>
       </c>
       <c r="FB52" s="13">
-        <f t="shared" si="61"/>
+        <f t="shared" si="64"/>
         <v>34</v>
       </c>
       <c r="FC52" s="45" t="s">
@@ -38186,8 +38363,24 @@
         <v>5</v>
       </c>
       <c r="FE52" s="152">
-        <f t="shared" ref="FE52:FE55" si="62">FD52/$FD$56</f>
+        <f t="shared" ref="FE52:FE55" si="65">FD52/$FD$56</f>
         <v>0.11363636363636363</v>
+      </c>
+      <c r="FF52" s="6">
+        <f>COUNTIF(FF$4:FF$47,3)</f>
+        <v>7</v>
+      </c>
+      <c r="FG52" s="6">
+        <f t="shared" ref="FG52:FI52" si="66">COUNTIF(FG$4:FG$47,3)</f>
+        <v>17</v>
+      </c>
+      <c r="FH52" s="6">
+        <f t="shared" si="66"/>
+        <v>13</v>
+      </c>
+      <c r="FI52" s="6">
+        <f t="shared" si="66"/>
+        <v>7</v>
       </c>
     </row>
     <row r="53" spans="1:165" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
@@ -38204,460 +38397,460 @@
         <v>9.7272727272727266</v>
       </c>
       <c r="R53" s="139" t="e">
-        <f t="shared" ref="R53:CC53" si="63">AVERAGE(R4:R47)</f>
+        <f t="shared" ref="R53:CC53" si="67">AVERAGE(R4:R47)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.1590909090909092</v>
       </c>
       <c r="T53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.25</v>
       </c>
       <c r="U53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.5681818181818183</v>
       </c>
       <c r="W53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>9.9772727272727266</v>
       </c>
       <c r="X53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.5454545454545454</v>
       </c>
       <c r="Y53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.9545454545454546</v>
       </c>
       <c r="AA53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>5.5</v>
       </c>
       <c r="AB53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.8409090909090908</v>
       </c>
       <c r="AD53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.6818181818181817</v>
       </c>
       <c r="AF53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>7.5227272727272725</v>
       </c>
       <c r="AG53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>32.727272727272727</v>
       </c>
       <c r="AH53" s="139"/>
       <c r="AI53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.0681818181818183</v>
       </c>
       <c r="AJ53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.0681818181818183</v>
       </c>
       <c r="AK53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AL53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.9318181818181817</v>
       </c>
       <c r="AM53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>9.0681818181818183</v>
       </c>
       <c r="AN53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.3863636363636362</v>
       </c>
       <c r="AO53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AP53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.4318181818181817</v>
       </c>
       <c r="AQ53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>6.8181818181818183</v>
       </c>
       <c r="AR53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.5227272727272729</v>
       </c>
       <c r="AS53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.4545454545454546</v>
       </c>
       <c r="AT53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.5454545454545454</v>
       </c>
       <c r="AU53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>5.0681818181818183</v>
       </c>
       <c r="AV53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.4090909090909092</v>
       </c>
       <c r="AW53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.1818181818181817</v>
       </c>
       <c r="AX53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AY53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.0909090909090908</v>
       </c>
       <c r="AZ53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>8.6818181818181817</v>
       </c>
       <c r="BA53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>29.636363636363637</v>
       </c>
       <c r="BB53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.5454545454545454</v>
       </c>
       <c r="BC53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BD53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.3409090909090908</v>
       </c>
       <c r="BE53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BF53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.4318181818181817</v>
       </c>
       <c r="BG53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>10.318181818181818</v>
       </c>
       <c r="BH53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BI53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.25</v>
       </c>
       <c r="BJ53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.5454545454545454</v>
       </c>
       <c r="BK53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.8863636363636362</v>
       </c>
       <c r="BL53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>8.6818181818181817</v>
       </c>
       <c r="BM53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.7272727272727271</v>
       </c>
       <c r="BN53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.8181818181818183</v>
       </c>
       <c r="BO53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>5.5454545454545459</v>
       </c>
       <c r="BP53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.0909090909090908</v>
       </c>
       <c r="BQ53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BR53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.4090909090909092</v>
       </c>
       <c r="BS53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>6.5</v>
       </c>
       <c r="BT53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>31.045454545454547</v>
       </c>
       <c r="BU53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.0227272727272729</v>
       </c>
       <c r="BV53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.0909090909090908</v>
       </c>
       <c r="BW53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>6.1136363636363633</v>
       </c>
       <c r="BX53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BY53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.2727272727272729</v>
       </c>
       <c r="BZ53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>3.25</v>
       </c>
       <c r="CA53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>2.8409090909090908</v>
       </c>
       <c r="CB53" s="139">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>9.3636363636363633</v>
       </c>
       <c r="CC53" s="139" t="e">
-        <f t="shared" si="63"/>
+        <f t="shared" si="67"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CD53" s="139">
-        <f t="shared" ref="CD53:EB53" si="64">AVERAGE(CD4:CD47)</f>
+        <f t="shared" ref="CD53:EB53" si="68">AVERAGE(CD4:CD47)</f>
         <v>3.0681818181818183</v>
       </c>
       <c r="CE53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.1818181818181817</v>
       </c>
       <c r="CF53" s="139" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CG53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.0227272727272729</v>
       </c>
       <c r="CH53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>9.2727272727272734</v>
       </c>
       <c r="CI53" s="139" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CJ53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.9772727272727271</v>
       </c>
       <c r="CK53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.5</v>
       </c>
       <c r="CL53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>7.4772727272727275</v>
       </c>
       <c r="CM53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>32.227272727272727</v>
       </c>
       <c r="CN53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.7272727272727271</v>
       </c>
       <c r="CO53" s="139" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CP53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.5454545454545454</v>
       </c>
       <c r="CQ53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>7.2727272727272725</v>
       </c>
       <c r="CR53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.7954545454545454</v>
       </c>
       <c r="CS53" s="139" t="e">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CT53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>4.0227272727272725</v>
       </c>
       <c r="CU53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>7.8181818181818183</v>
       </c>
       <c r="CV53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.9090909090909092</v>
       </c>
       <c r="CW53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>4.0909090909090908</v>
       </c>
       <c r="CX53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.7727272727272729</v>
       </c>
       <c r="CY53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.9090909090909092</v>
       </c>
       <c r="CZ53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>10.772727272727273</v>
       </c>
       <c r="DA53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.1363636363636362</v>
       </c>
       <c r="DB53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.8636363636363638</v>
       </c>
       <c r="DC53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.1363636363636362</v>
       </c>
       <c r="DD53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.8636363636363638</v>
       </c>
       <c r="DE53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.2954545454545454</v>
       </c>
       <c r="DF53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.7045454545454546</v>
       </c>
       <c r="DG53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>11.431818181818182</v>
       </c>
       <c r="DH53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>37.295454545454547</v>
       </c>
       <c r="DI53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.3863636363636362</v>
       </c>
       <c r="DJ53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.6136363636363638</v>
       </c>
       <c r="DK53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.2954545454545454</v>
       </c>
       <c r="DL53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>6.9090909090909092</v>
       </c>
       <c r="DM53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.5909090909090908</v>
       </c>
       <c r="DN53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.1590909090909092</v>
       </c>
       <c r="DO53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.8409090909090908</v>
       </c>
       <c r="DP53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>7.4318181818181817</v>
       </c>
       <c r="DQ53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.4090909090909092</v>
       </c>
       <c r="DR53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.6590909090909092</v>
       </c>
       <c r="DS53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.8863636363636362</v>
       </c>
       <c r="DT53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.1136363636363638</v>
       </c>
       <c r="DU53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>10.181818181818182</v>
       </c>
       <c r="DV53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>1.8863636363636365</v>
       </c>
       <c r="DW53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>4.1136363636363633</v>
       </c>
       <c r="DX53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.5909090909090908</v>
       </c>
       <c r="DY53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>2.4318181818181817</v>
       </c>
       <c r="DZ53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>3.5681818181818183</v>
       </c>
       <c r="EA53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>11.272727272727273</v>
       </c>
       <c r="EB53" s="139">
-        <f t="shared" si="64"/>
+        <f t="shared" si="68"/>
         <v>35.795454545454547</v>
       </c>
       <c r="ED53"/>
@@ -38666,47 +38859,47 @@
         <v>0.79545454545454541</v>
       </c>
       <c r="EF53" s="151">
-        <f t="shared" ref="EF53:EP53" si="65">(EF51/(EF51+EF52))</f>
+        <f t="shared" ref="EF53:EP53" si="69">(EF51/(EF51+EF52))</f>
         <v>0.59090909090909094</v>
       </c>
       <c r="EG53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.36363636363636365</v>
       </c>
       <c r="EH53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.59090909090909094</v>
       </c>
       <c r="EI53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.43181818181818182</v>
       </c>
       <c r="EJ53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.65909090909090906</v>
       </c>
       <c r="EK53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.54545454545454541</v>
       </c>
       <c r="EL53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.11363636363636363</v>
       </c>
       <c r="EM53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.38636363636363635</v>
       </c>
       <c r="EN53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.31818181818181818</v>
       </c>
       <c r="EO53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.52272727272727271</v>
       </c>
       <c r="EP53" s="151">
-        <f t="shared" si="65"/>
+        <f t="shared" si="69"/>
         <v>0.29545454545454547</v>
       </c>
       <c r="EQ53"/>
@@ -38715,43 +38908,43 @@
         <v>0.65909090909090906</v>
       </c>
       <c r="ES53" s="151">
-        <f t="shared" ref="ES53:FB53" si="66">(ES51/(ES51+ES52))</f>
+        <f t="shared" ref="ES53:FB53" si="70">(ES51/(ES51+ES52))</f>
         <v>0.59090909090909094</v>
       </c>
       <c r="ET53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.5</v>
       </c>
       <c r="EU53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.61363636363636365</v>
       </c>
       <c r="EV53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.38636363636363635</v>
       </c>
       <c r="EW53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.29545454545454547</v>
       </c>
       <c r="EX53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.29545454545454547</v>
       </c>
       <c r="EY53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.13636363636363635</v>
       </c>
       <c r="EZ53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.27272727272727271</v>
       </c>
       <c r="FA53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.52272727272727271</v>
       </c>
       <c r="FB53" s="151">
-        <f t="shared" si="66"/>
+        <f t="shared" si="70"/>
         <v>0.22727272727272727</v>
       </c>
       <c r="FC53" s="143" t="s">
@@ -38762,8 +38955,24 @@
         <v>10</v>
       </c>
       <c r="FE53" s="152">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>0.22727272727272727</v>
+      </c>
+      <c r="FF53" s="6">
+        <f>COUNTIF(FF$4:FF$47,2)</f>
+        <v>10</v>
+      </c>
+      <c r="FG53" s="6">
+        <f t="shared" ref="FG53:FI53" si="71">COUNTIF(FG$4:FG$47,2)</f>
+        <v>9</v>
+      </c>
+      <c r="FH53" s="6">
+        <f t="shared" si="71"/>
+        <v>12</v>
+      </c>
+      <c r="FI53" s="6">
+        <f t="shared" si="71"/>
+        <v>13</v>
       </c>
     </row>
     <row r="54" spans="1:165" s="13" customFormat="1" ht="15.75" customHeight="1" thickBot="1">
@@ -38835,8 +39044,24 @@
         <v>6</v>
       </c>
       <c r="FE54" s="152">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>0.13636363636363635</v>
+      </c>
+      <c r="FF54" s="6">
+        <f>COUNTIF(FF$4:FF$47,1)</f>
+        <v>14</v>
+      </c>
+      <c r="FG54" s="6">
+        <f t="shared" ref="FG54:FI54" si="72">COUNTIF(FG$4:FG$47,1)</f>
+        <v>5</v>
+      </c>
+      <c r="FH54" s="6">
+        <f t="shared" si="72"/>
+        <v>6</v>
+      </c>
+      <c r="FI54" s="6">
+        <f t="shared" si="72"/>
+        <v>19</v>
       </c>
     </row>
     <row r="55" spans="1:165" s="13" customFormat="1" ht="15.75" customHeight="1">
@@ -38984,7 +39209,7 @@
         <v>3</v>
       </c>
       <c r="FE55" s="152">
-        <f t="shared" si="62"/>
+        <f t="shared" si="65"/>
         <v>6.8181818181818177E-2</v>
       </c>
     </row>
@@ -39070,460 +39295,460 @@
         <v>2.9520480581866475</v>
       </c>
       <c r="R57" s="11" t="e">
-        <f t="shared" ref="R57:CC57" si="67">_xlfn.STDEV.S(R$4:R$47)</f>
+        <f t="shared" ref="R57:CC57" si="73">_xlfn.STDEV.S(R$4:R$47)</f>
         <v>#DIV/0!</v>
       </c>
       <c r="S57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.3967267685420599</v>
       </c>
       <c r="T57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1837072233866255</v>
       </c>
       <c r="U57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="V57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.4042746579677958</v>
       </c>
       <c r="W57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>3.3652715869781784</v>
       </c>
       <c r="X57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.0880865529557127</v>
       </c>
       <c r="Y57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="Z57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2750658068661884</v>
       </c>
       <c r="AA57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.9824814143238607</v>
       </c>
       <c r="AB57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AC57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.0552897060221724</v>
       </c>
       <c r="AD57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AE57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.0734150516692529</v>
       </c>
       <c r="AF57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.8861630347500453</v>
       </c>
       <c r="AG57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>7.4470647764307225</v>
       </c>
       <c r="AH57" s="11"/>
       <c r="AI57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2648692785243687</v>
       </c>
       <c r="AJ57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1080619425370331</v>
       </c>
       <c r="AK57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AL57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1492713014396978</v>
       </c>
       <c r="AM57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.9095564719750324</v>
       </c>
       <c r="AN57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2240973720751764</v>
       </c>
       <c r="AO57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AP57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1693314980021159</v>
       </c>
       <c r="AQ57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>2.2232673135654895</v>
       </c>
       <c r="AR57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.0227331453907034</v>
       </c>
       <c r="AS57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>0.87483009525293132</v>
       </c>
       <c r="AT57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>0.87483009525293209</v>
       </c>
       <c r="AU57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.5759489909217601</v>
       </c>
       <c r="AV57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1063911966006568</v>
       </c>
       <c r="AW57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1467391032072312</v>
       </c>
       <c r="AX57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="AY57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2907214823623694</v>
       </c>
       <c r="AZ57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>2.6656534368224105</v>
       </c>
       <c r="BA57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>5.6407607481776578</v>
       </c>
       <c r="BB57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2474074594850142</v>
       </c>
       <c r="BC57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BD57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1400363482206479</v>
       </c>
       <c r="BE57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BF57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.4370144643755411</v>
       </c>
       <c r="BG57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>3.2762196541116295</v>
       </c>
       <c r="BH57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BI57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.399750808387477</v>
       </c>
       <c r="BJ57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2474074594850149</v>
       </c>
       <c r="BK57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2615219507148128</v>
       </c>
       <c r="BL57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>3.4084213577871902</v>
       </c>
       <c r="BM57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2457114594355845</v>
       </c>
       <c r="BN57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2808559505945085</v>
       </c>
       <c r="BO57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>2.1615513965081425</v>
       </c>
       <c r="BP57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.3086151355301867</v>
       </c>
       <c r="BQ57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BR57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2069215465183796</v>
       </c>
       <c r="BS57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>2.1185778468168821</v>
       </c>
       <c r="BT57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>9.6856512080224721</v>
       </c>
       <c r="BU57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2665396249484193</v>
       </c>
       <c r="BV57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.1374835918710644</v>
       </c>
       <c r="BW57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>2.1804193013752484</v>
       </c>
       <c r="BX57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="BY57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.2269007344777967</v>
       </c>
       <c r="BZ57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.0810201899885084</v>
       </c>
       <c r="CA57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>1.0771016625849856</v>
       </c>
       <c r="CB57" s="11">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>2.694446563451963</v>
       </c>
       <c r="CC57" s="11" t="e">
-        <f t="shared" si="67"/>
+        <f t="shared" si="73"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CD57" s="11">
-        <f t="shared" ref="CD57:EB57" si="68">_xlfn.STDEV.S(CD$4:CD$47)</f>
+        <f t="shared" ref="CD57:EB57" si="74">_xlfn.STDEV.S(CD$4:CD$47)</f>
         <v>1.2648692785243687</v>
       </c>
       <c r="CE57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.2060453783110545</v>
       </c>
       <c r="CF57" s="11" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CG57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.0227331453907034</v>
       </c>
       <c r="CH57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>2.8314154268208145</v>
       </c>
       <c r="CI57" s="11" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CJ57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.0888149385463499</v>
       </c>
       <c r="CK57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.1102063499795358</v>
       </c>
       <c r="CL57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.9468356718512183</v>
       </c>
       <c r="CM57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>7.5355394750279157</v>
       </c>
       <c r="CN57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.1281521496355327</v>
       </c>
       <c r="CO57" s="11" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CP57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.1704609597722389</v>
       </c>
       <c r="CQ57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.7961669312233457</v>
       </c>
       <c r="CR57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.1926040582466166</v>
       </c>
       <c r="CS57" s="11" t="e">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>#DIV/0!</v>
       </c>
       <c r="CT57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.9273276524793459</v>
       </c>
       <c r="CU57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.8460860832145605</v>
       </c>
       <c r="CV57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.0958310389662929</v>
       </c>
       <c r="CW57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.0958310389662929</v>
       </c>
       <c r="CX57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.93668481119209512</v>
       </c>
       <c r="CY57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.2354865686484746</v>
       </c>
       <c r="CZ57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>2.3709838637218947</v>
       </c>
       <c r="DA57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.904534033733291</v>
       </c>
       <c r="DB57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.90453403373329022</v>
       </c>
       <c r="DC57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.0250560754010982</v>
       </c>
       <c r="DD57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.0250560754010976</v>
       </c>
       <c r="DE57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.9783599341124577</v>
       </c>
       <c r="DF57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.97835993411245736</v>
       </c>
       <c r="DG57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>2.0842457480504533</v>
       </c>
       <c r="DH57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>5.5008648176511139</v>
       </c>
       <c r="DI57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.2240973720751764</v>
       </c>
       <c r="DJ57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.224097372075176</v>
       </c>
       <c r="DK57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.322076334821533</v>
       </c>
       <c r="DL57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>2.2080000612801407</v>
       </c>
       <c r="DM57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.2069215465183796</v>
       </c>
       <c r="DN57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.1801297094295287</v>
       </c>
       <c r="DO57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.1801297094295287</v>
       </c>
       <c r="DP57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>2.061809177022071</v>
       </c>
       <c r="DQ57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.3523138107355597</v>
       </c>
       <c r="DR57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.1602562230693905</v>
       </c>
       <c r="DS57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.2798239175926833</v>
       </c>
       <c r="DT57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.2798239175926833</v>
       </c>
       <c r="DU57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>2.8224410288830142</v>
       </c>
       <c r="DV57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.92046270191881141</v>
       </c>
       <c r="DW57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.92046270191881074</v>
       </c>
       <c r="DX57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>0.84408149662143939</v>
       </c>
       <c r="DY57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.3707530992839732</v>
       </c>
       <c r="DZ57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>1.3707530992839725</v>
       </c>
       <c r="EA57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>2.3660745271601473</v>
       </c>
       <c r="EB57" s="11">
-        <f t="shared" si="68"/>
+        <f t="shared" si="74"/>
         <v>7.5346626765269704</v>
       </c>
       <c r="ED57" s="6"/>
@@ -39606,6 +39831,25 @@
       <c r="EB58" s="42"/>
       <c r="ED58"/>
       <c r="EQ58"/>
+      <c r="FE58" s="13" t="s">
+        <v>444</v>
+      </c>
+      <c r="FF58" s="170">
+        <f>(FF51+FF52)/(FF51+FF52+FF53+FF54)</f>
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="FG58" s="170">
+        <f t="shared" ref="FG58:FI58" si="75">(FG51+FG52)/(FG51+FG52+FG53+FG54)</f>
+        <v>0.68181818181818177</v>
+      </c>
+      <c r="FH58" s="170">
+        <f t="shared" si="75"/>
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="FI58" s="170">
+        <f t="shared" si="75"/>
+        <v>0.27272727272727271</v>
+      </c>
     </row>
     <row r="59" spans="1:165" s="13" customFormat="1" ht="15.75" customHeight="1">
       <c r="B59" s="11"/>
@@ -39699,6 +39943,25 @@
       <c r="EM59" s="105"/>
       <c r="EN59" s="105"/>
       <c r="EQ59"/>
+      <c r="FE59" s="13" t="s">
+        <v>445</v>
+      </c>
+      <c r="FF59" s="170">
+        <f>(FF53+FF54)/(FF51+FF52+FF53+FF54)</f>
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="FG59" s="170">
+        <f t="shared" ref="FG59:FI59" si="76">(FG53+FG54)/(FG51+FG52+FG53+FG54)</f>
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="FH59" s="170">
+        <f t="shared" si="76"/>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="FI59" s="170">
+        <f t="shared" si="76"/>
+        <v>0.72727272727272729</v>
+      </c>
     </row>
     <row r="60" spans="1:165" s="13" customFormat="1" ht="33" customHeight="1">
       <c r="B60" s="11"/>
@@ -40098,43 +40361,43 @@
         <v>-6.8758888798753854E-3</v>
       </c>
       <c r="ES62" s="86">
-        <f t="shared" ref="ES62:FB62" si="69">CORREL($EB4:$EB47,ES4:ES47)</f>
+        <f t="shared" ref="ES62:FB62" si="77">CORREL($EB4:$EB47,ES4:ES47)</f>
         <v>-0.13455538035361217</v>
       </c>
       <c r="ET62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>-1.5256173687248702E-2</v>
       </c>
       <c r="EU62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>9.7272478306481433E-2</v>
       </c>
       <c r="EV62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>0.24738256928017316</v>
       </c>
       <c r="EW62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>7.1284636555403569E-2</v>
       </c>
       <c r="EX62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>-9.5907474768570658E-2</v>
       </c>
       <c r="EY62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>-7.8000161377933766E-2</v>
       </c>
       <c r="EZ62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>-0.11335518424847073</v>
       </c>
       <c r="FA62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>0.20589376995673844</v>
       </c>
       <c r="FB62" s="86">
-        <f t="shared" si="69"/>
+        <f t="shared" si="77"/>
         <v>-0.13072638533016404</v>
       </c>
       <c r="FC62" s="86"/>
@@ -40146,15 +40409,15 @@
         <v>-0.12600436939298465</v>
       </c>
       <c r="FG62" s="86">
-        <f t="shared" ref="FG62:FI62" si="70">CORREL($EB4:$EB47,FG4:FG47)</f>
+        <f t="shared" ref="FG62:FI62" si="78">CORREL($EB4:$EB47,FG4:FG47)</f>
         <v>-6.3794983585467369E-2</v>
       </c>
       <c r="FH62" s="86">
-        <f t="shared" si="70"/>
+        <f t="shared" si="78"/>
         <v>0.11234740504733795</v>
       </c>
       <c r="FI62" s="86">
-        <f t="shared" si="70"/>
+        <f t="shared" si="78"/>
         <v>9.7352943401443223E-2</v>
       </c>
     </row>
@@ -40287,47 +40550,47 @@
         <v>275</v>
       </c>
       <c r="ER63" s="164">
-        <f t="shared" ref="EQ63:FB63" si="71">CORREL($DH4:$DH47,ER4:ER47)</f>
+        <f t="shared" ref="EQ63:FB63" si="79">CORREL($DH4:$DH47,ER4:ER47)</f>
         <v>0.32121613740289029</v>
       </c>
       <c r="ES63" s="86">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>1.9705420497446245E-2</v>
       </c>
       <c r="ET63" s="164">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>0.33016843627303538</v>
       </c>
       <c r="EU63" s="164">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>0.30061092331008604</v>
       </c>
       <c r="EV63" s="86">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>0.19722105351492333</v>
       </c>
       <c r="EW63" s="86">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>0.12054092011793432</v>
       </c>
       <c r="EX63" s="86">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>1.9777871176517713E-2</v>
       </c>
       <c r="EY63" s="157">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>-0.27733760422750248</v>
       </c>
       <c r="EZ63" s="158">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>0.45470533497484411</v>
       </c>
       <c r="FA63" s="86">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>0.18579304815596498</v>
       </c>
       <c r="FB63" s="86">
-        <f t="shared" si="71"/>
+        <f t="shared" si="79"/>
         <v>-0.16908607015295132</v>
       </c>
       <c r="FC63" s="86"/>
@@ -40335,19 +40598,19 @@
         <v>275</v>
       </c>
       <c r="FF63" s="86">
-        <f t="shared" ref="FF63:FI63" si="72">CORREL($DH4:$DH47,FF4:FF47)</f>
+        <f t="shared" ref="FF63:FI63" si="80">CORREL($DH4:$DH47,FF4:FF47)</f>
         <v>-8.1325248774302944E-2</v>
       </c>
       <c r="FG63" s="86">
-        <f t="shared" si="72"/>
+        <f t="shared" si="80"/>
         <v>0.11133774460363048</v>
       </c>
       <c r="FH63" s="86">
-        <f t="shared" si="72"/>
+        <f t="shared" si="80"/>
         <v>-0.13757917740149953</v>
       </c>
       <c r="FI63" s="86">
-        <f t="shared" si="72"/>
+        <f t="shared" si="80"/>
         <v>0.12925506699197747</v>
       </c>
     </row>
@@ -40480,47 +40743,47 @@
         <v>274</v>
       </c>
       <c r="ER64" s="86">
-        <f t="shared" ref="EQ64:FB64" si="73">CORREL($CM4:$CM47,ER4:ER47)</f>
+        <f t="shared" ref="EQ64:FB64" si="81">CORREL($CM4:$CM47,ER4:ER47)</f>
         <v>-4.2420760897363227E-2</v>
       </c>
       <c r="ES64" s="164">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>-0.32210558695379504</v>
       </c>
       <c r="ET64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>1.8305278264234667E-2</v>
       </c>
       <c r="EU64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>0.16205446597148021</v>
       </c>
       <c r="EV64" s="164">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>-0.3249633491624937</v>
       </c>
       <c r="EW64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>-0.12006036323428609</v>
       </c>
       <c r="EX64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>-6.3829560200506221E-3</v>
       </c>
       <c r="EY64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>5.8998437857408423E-2</v>
       </c>
       <c r="EZ64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>0.11832406049911934</v>
       </c>
       <c r="FA64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>-0.10522543383625724</v>
       </c>
       <c r="FB64" s="86">
-        <f t="shared" si="73"/>
+        <f t="shared" si="81"/>
         <v>-9.2656022535027322E-3</v>
       </c>
       <c r="FC64" s="86"/>
@@ -40528,19 +40791,19 @@
         <v>274</v>
       </c>
       <c r="FF64" s="86">
-        <f t="shared" ref="FF64:FI64" si="74">CORREL($CM4:$CM47,FF4:FF47)</f>
+        <f t="shared" ref="FF64:FI64" si="82">CORREL($CM4:$CM47,FF4:FF47)</f>
         <v>-9.1306827033789673E-2</v>
       </c>
       <c r="FG64" s="86">
-        <f t="shared" si="74"/>
+        <f t="shared" si="82"/>
         <v>-0.15968391603293175</v>
       </c>
       <c r="FH64" s="86">
-        <f t="shared" si="74"/>
+        <f t="shared" si="82"/>
         <v>-1.4878719583180334E-3</v>
       </c>
       <c r="FI64" s="157">
-        <f t="shared" si="74"/>
+        <f t="shared" si="82"/>
         <v>0.26120679075457692</v>
       </c>
     </row>
@@ -40728,15 +40991,15 @@
         <v>0.12936148392201219</v>
       </c>
       <c r="FG65" s="89">
-        <f t="shared" ref="FG65:FI65" si="75">CORREL($BT4:$BT47,FG4:FG47)</f>
+        <f t="shared" ref="FG65:FI65" si="83">CORREL($BT4:$BT47,FG4:FG47)</f>
         <v>1.2936580539860805E-2</v>
       </c>
       <c r="FH65" s="89">
-        <f t="shared" si="75"/>
+        <f t="shared" si="83"/>
         <v>-0.22804329560020592</v>
       </c>
       <c r="FI65" s="89">
-        <f t="shared" si="75"/>
+        <f t="shared" si="83"/>
         <v>6.2952238711127803E-2</v>
       </c>
     </row>
@@ -40872,47 +41135,47 @@
         <v>256</v>
       </c>
       <c r="ER66" s="86">
-        <f t="shared" ref="EQ66:FB66" si="76">CORREL($BA4:$BA47,ER4:ER47)</f>
+        <f t="shared" ref="EQ66:FB66" si="84">CORREL($BA4:$BA47,ER4:ER47)</f>
         <v>3.9082930608199631E-2</v>
       </c>
       <c r="ES66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.15298007062213423</v>
       </c>
       <c r="ET66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.1304222633502756</v>
       </c>
       <c r="EU66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>7.3812027894479063E-2</v>
       </c>
       <c r="EV66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.12707843977709277</v>
       </c>
       <c r="EW66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.14049320687741904</v>
       </c>
       <c r="EX66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>-1.1369392464068579E-2</v>
       </c>
       <c r="EY66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>-0.16411108249464351</v>
       </c>
       <c r="EZ66" s="157">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.28702202793213005</v>
       </c>
       <c r="FA66" s="158">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>0.39463882793808647</v>
       </c>
       <c r="FB66" s="86">
-        <f t="shared" si="76"/>
+        <f t="shared" si="84"/>
         <v>-0.18832236114194667</v>
       </c>
       <c r="FC66" s="86"/>
@@ -40920,19 +41183,19 @@
         <v>256</v>
       </c>
       <c r="FF66" s="86">
-        <f t="shared" ref="FF66:FI66" si="77">CORREL($BA4:$BA47,FF4:FF47)</f>
+        <f t="shared" ref="FF66:FI66" si="85">CORREL($BA4:$BA47,FF4:FF47)</f>
         <v>-2.0456811329673519E-2</v>
       </c>
       <c r="FG66" s="86">
-        <f t="shared" si="77"/>
+        <f t="shared" si="85"/>
         <v>0.1087679614743388</v>
       </c>
       <c r="FH66" s="86">
-        <f t="shared" si="77"/>
+        <f t="shared" si="85"/>
         <v>-0.10335835103880273</v>
       </c>
       <c r="FI66" s="86">
-        <f t="shared" si="77"/>
+        <f t="shared" si="85"/>
         <v>2.5028518978907954E-2</v>
       </c>
     </row>
@@ -41068,47 +41331,47 @@
         <v>237</v>
       </c>
       <c r="ER67" s="86">
-        <f t="shared" ref="EQ67:FB67" si="78">CORREL($AG4:$AG47,ER4:ER47)</f>
+        <f t="shared" ref="EQ67:FB67" si="86">CORREL($AG4:$AG47,ER4:ER47)</f>
         <v>8.4073283602049576E-2</v>
       </c>
       <c r="ES67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>-0.20035421514883298</v>
       </c>
       <c r="ET67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>2.4697004990579873E-2</v>
       </c>
       <c r="EU67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>0.11642850488561288</v>
       </c>
       <c r="EV67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>0.23228063103416821</v>
       </c>
       <c r="EW67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>-0.12486991286839574</v>
       </c>
       <c r="EX67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>-0.17223436257709754</v>
       </c>
       <c r="EY67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>5.7245968907085098E-3</v>
       </c>
       <c r="EZ67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>-0.12981231711238966</v>
       </c>
       <c r="FA67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>0.10675650057961095</v>
       </c>
       <c r="FB67" s="86">
-        <f t="shared" si="78"/>
+        <f t="shared" si="86"/>
         <v>0.13795646443342033</v>
       </c>
       <c r="FC67" s="86"/>
@@ -41117,19 +41380,19 @@
         <v>237</v>
       </c>
       <c r="FF67" s="86">
-        <f t="shared" ref="FF67:FI67" si="79">CORREL($AG4:$AG47,FF4:FF47)</f>
+        <f t="shared" ref="FF67:FI67" si="87">CORREL($AG4:$AG47,FF4:FF47)</f>
         <v>-1.2257207966486716E-2</v>
       </c>
       <c r="FG67" s="86">
-        <f t="shared" si="79"/>
+        <f t="shared" si="87"/>
         <v>-0.2158281721522308</v>
       </c>
       <c r="FH67" s="86">
-        <f t="shared" si="79"/>
+        <f t="shared" si="87"/>
         <v>-3.0110971805100291E-3</v>
       </c>
       <c r="FI67" s="86">
-        <f t="shared" si="79"/>
+        <f t="shared" si="87"/>
         <v>0.22199846414960164</v>
       </c>
     </row>
@@ -41479,55 +41742,55 @@
         <v>-1.6638644275632388</v>
       </c>
       <c r="ED71" s="13">
-        <f t="shared" ref="ED71:EP71" si="80">(ED62*SQRT(44-2))/(SQRT(1-ED62^2))</f>
+        <f t="shared" ref="ED71:EP71" si="88">(ED62*SQRT(44-2))/(SQRT(1-ED62^2))</f>
         <v>0</v>
       </c>
       <c r="EE71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>1.7879897119581536</v>
       </c>
       <c r="EF71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>2.516055042872186</v>
       </c>
       <c r="EG71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>1.0524925503960214</v>
       </c>
       <c r="EH71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>-1.9158741837786406</v>
       </c>
       <c r="EI71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>-1.181412247250005</v>
       </c>
       <c r="EJ71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>2.7099226329209349</v>
       </c>
       <c r="EK71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>2.6072990320446863</v>
       </c>
       <c r="EL71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>-0.81494042014697587</v>
       </c>
       <c r="EM71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>0.26326724574097438</v>
       </c>
       <c r="EN71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>-9.0708087315529207E-2</v>
       </c>
       <c r="EO71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>1.2793898498491825</v>
       </c>
       <c r="EP71" s="13">
-        <f t="shared" si="80"/>
+        <f t="shared" si="88"/>
         <v>1.3576448178931135</v>
       </c>
       <c r="EQ71" s="17" t="s">
@@ -41538,43 +41801,43 @@
         <v>-4.4561906309503366E-2</v>
       </c>
       <c r="ES71" s="13">
-        <f t="shared" ref="ES71:FB71" si="81">(ES62*SQRT(44-2))/(SQRT(1-ES62^2))</f>
+        <f t="shared" ref="ES71:FB71" si="89">(ES62*SQRT(44-2))/(SQRT(1-ES62^2))</f>
         <v>-0.8800213779924374</v>
       </c>
       <c r="ET71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>-9.8882813915387877E-2</v>
       </c>
       <c r="EU71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>0.63340143274706961</v>
       </c>
       <c r="EV71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>1.6546523834288978</v>
       </c>
       <c r="EW71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>0.46315550625089569</v>
       </c>
       <c r="EX71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>-0.62442993888982423</v>
       </c>
       <c r="EY71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>-0.50704360657227654</v>
       </c>
       <c r="EZ71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>-0.73939128095359397</v>
       </c>
       <c r="FA71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>1.3635592804847947</v>
       </c>
       <c r="FB71" s="13">
-        <f t="shared" si="81"/>
+        <f t="shared" si="89"/>
         <v>-0.8545370281856971</v>
       </c>
       <c r="FE71" s="17" t="s">
@@ -41585,15 +41848,15 @@
         <v>-0.8231625081551921</v>
       </c>
       <c r="FG71" s="13">
-        <f t="shared" ref="FG71:FI71" si="82">(FG62*SQRT(44-2))/(SQRT(1-FG62^2))</f>
+        <f t="shared" ref="FG71:FI71" si="90">(FG62*SQRT(44-2))/(SQRT(1-FG62^2))</f>
         <v>-0.4142826296696675</v>
       </c>
       <c r="FH71" s="13">
-        <f t="shared" si="82"/>
+        <f t="shared" si="90"/>
         <v>0.73273334277997071</v>
       </c>
       <c r="FI71" s="13">
-        <f t="shared" si="82"/>
+        <f t="shared" si="90"/>
         <v>0.63393040216967811</v>
       </c>
     </row>
@@ -41675,125 +41938,125 @@
         <v>275</v>
       </c>
       <c r="EC72" s="13">
-        <f t="shared" ref="EC72:EP76" si="83">(EC63*SQRT(44-2))/(SQRT(1-EC63^2))</f>
+        <f t="shared" ref="EC72:EP76" si="91">(EC63*SQRT(44-2))/(SQRT(1-EC63^2))</f>
         <v>-0.83107291618354995</v>
       </c>
       <c r="ED72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="EE72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>2.3304578233743896</v>
       </c>
       <c r="EF72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.85110534453149245</v>
       </c>
       <c r="EG72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.58072317471973078</v>
       </c>
       <c r="EH72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.62641020957173499</v>
       </c>
       <c r="EI72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.1889516970609444</v>
       </c>
       <c r="EJ72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.4911474021082662</v>
       </c>
       <c r="EK72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.37645889382244602</v>
       </c>
       <c r="EL72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.1260989158662289</v>
       </c>
       <c r="EM72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.67236836839556113</v>
       </c>
       <c r="EN72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.69383106010732376</v>
       </c>
       <c r="EO72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.6928450962925021</v>
       </c>
       <c r="EP72" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.5348972353258326</v>
       </c>
       <c r="EQ72" s="17" t="s">
         <v>275</v>
       </c>
       <c r="ER72" s="13">
-        <f t="shared" ref="ER72:FB72" si="84">(ER63*SQRT(44-2))/(SQRT(1-ER63^2))</f>
+        <f t="shared" ref="ER72:FB72" si="92">(ER63*SQRT(44-2))/(SQRT(1-ER63^2))</f>
         <v>2.1982106692829659</v>
       </c>
       <c r="ES72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>0.12773052211549468</v>
       </c>
       <c r="ET72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>2.266856740611197</v>
       </c>
       <c r="EU72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>2.0426609271008389</v>
       </c>
       <c r="EV72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>1.3037453118043711</v>
       </c>
       <c r="EW72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>0.7869324757185483</v>
       </c>
       <c r="EX72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>0.12820033080315568</v>
       </c>
       <c r="EY72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>-1.8707373950499102</v>
       </c>
       <c r="EZ72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>3.3086555333878271</v>
       </c>
       <c r="FA72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>1.2254123475519894</v>
       </c>
       <c r="FB72" s="13">
-        <f t="shared" si="84"/>
+        <f t="shared" si="92"/>
         <v>-1.1118116307304058</v>
       </c>
       <c r="FE72" s="17" t="s">
         <v>275</v>
       </c>
       <c r="FF72" s="13">
-        <f t="shared" ref="FF72:FI72" si="85">(FF63*SQRT(44-2))/(SQRT(1-FF63^2))</f>
+        <f t="shared" ref="FF72:FI72" si="93">(FF63*SQRT(44-2))/(SQRT(1-FF63^2))</f>
         <v>-0.52879943632548676</v>
       </c>
       <c r="FG72" s="13">
-        <f t="shared" si="85"/>
+        <f t="shared" si="93"/>
         <v>0.72606527247562003</v>
       </c>
       <c r="FH72" s="13">
-        <f t="shared" si="85"/>
+        <f t="shared" si="93"/>
         <v>-0.90017494276996335</v>
       </c>
       <c r="FI72" s="13">
-        <f t="shared" si="85"/>
+        <f t="shared" si="93"/>
         <v>0.8447549015413931</v>
       </c>
     </row>
@@ -41875,125 +42138,125 @@
         <v>274</v>
       </c>
       <c r="EC73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.3246800470339466</v>
       </c>
       <c r="ED73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0</v>
       </c>
       <c r="EE73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.74230566180951463</v>
       </c>
       <c r="EF73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.69119526705717182</v>
       </c>
       <c r="EG73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.85555594621353437</v>
       </c>
       <c r="EH73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.60954728669348024</v>
       </c>
       <c r="EI73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.58846206207440832</v>
       </c>
       <c r="EJ73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.47718072710463394</v>
       </c>
       <c r="EK73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.73752950478866308</v>
       </c>
       <c r="EL73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.17847097108286392</v>
       </c>
       <c r="EM73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.1569349253602515</v>
       </c>
       <c r="EN73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.7508827929607935</v>
       </c>
       <c r="EO73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.18900795362203587</v>
       </c>
       <c r="EP73" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.21482864038172644</v>
       </c>
       <c r="EQ73" s="17" t="s">
         <v>274</v>
       </c>
       <c r="ER73" s="13">
-        <f t="shared" ref="ER73:FB73" si="86">(ER64*SQRT(44-2))/(SQRT(1-ER64^2))</f>
+        <f t="shared" ref="ER73:FB73" si="94">(ER64*SQRT(44-2))/(SQRT(1-ER64^2))</f>
         <v>-0.27516564626136547</v>
       </c>
       <c r="ES73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>-2.2050010743804256</v>
       </c>
       <c r="ET73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>0.11865164259504707</v>
       </c>
       <c r="EU73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>1.0643011020345003</v>
       </c>
       <c r="EV73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>-2.2268625828562802</v>
       </c>
       <c r="EW73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>-0.78374925926024419</v>
       </c>
       <c r="EX73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>-4.1367125556225945E-2</v>
       </c>
       <c r="EY73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>0.38302077081588703</v>
       </c>
       <c r="EZ73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>0.77225260331931866</v>
       </c>
       <c r="FA73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>-0.68574574183308323</v>
       </c>
       <c r="FB73" s="13">
-        <f t="shared" si="86"/>
+        <f t="shared" si="94"/>
         <v>-6.0050543386025591E-2</v>
       </c>
       <c r="FE73" s="17" t="s">
         <v>274</v>
       </c>
       <c r="FF73" s="13">
-        <f t="shared" ref="FF73:FI73" si="87">(FF64*SQRT(44-2))/(SQRT(1-FF64^2))</f>
+        <f t="shared" ref="FF73:FI73" si="95">(FF64*SQRT(44-2))/(SQRT(1-FF64^2))</f>
         <v>-0.59421803329145861</v>
       </c>
       <c r="FG73" s="13">
-        <f t="shared" si="87"/>
+        <f t="shared" si="95"/>
         <v>-1.0483219149817002</v>
       </c>
       <c r="FH73" s="13">
-        <f t="shared" si="87"/>
+        <f t="shared" si="95"/>
         <v>-9.642523027427569E-3</v>
       </c>
       <c r="FI73" s="13">
-        <f t="shared" si="87"/>
+        <f t="shared" si="95"/>
         <v>1.7536968055654349</v>
       </c>
     </row>
@@ -42075,125 +42338,125 @@
         <v>265</v>
       </c>
       <c r="EC74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.46115009132835999</v>
       </c>
       <c r="ED74" s="13" t="e">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>#DIV/0!</v>
       </c>
       <c r="EE74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.98001204298512024</v>
       </c>
       <c r="EF74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.43329573910761826</v>
       </c>
       <c r="EG74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.24728118850196218</v>
       </c>
       <c r="EH74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>5.6887787749961907E-2</v>
       </c>
       <c r="EI74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.68274777324352764</v>
       </c>
       <c r="EJ74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.6628079028518542</v>
       </c>
       <c r="EK74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.58655602825823328</v>
       </c>
       <c r="EL74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-1.5040463612692858</v>
       </c>
       <c r="EM74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-3.0253417421467441</v>
       </c>
       <c r="EN74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.4329163720542883</v>
       </c>
       <c r="EO74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.46172888191602307</v>
       </c>
       <c r="EP74" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.59559358808833562</v>
       </c>
       <c r="EQ74" s="17" t="s">
         <v>265</v>
       </c>
       <c r="ER74" s="13">
-        <f t="shared" ref="ER74:FB74" si="88">(ER65*SQRT(44-2))/(SQRT(1-ER65^2))</f>
+        <f t="shared" ref="ER74:FB74" si="96">(ER65*SQRT(44-2))/(SQRT(1-ER65^2))</f>
         <v>0.97405754280897416</v>
       </c>
       <c r="ES74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>-0.82577562694141893</v>
       </c>
       <c r="ET74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>-0.4626583315153594</v>
       </c>
       <c r="EU74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>2.7760560102217675</v>
       </c>
       <c r="EV74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>-1.2140879055747598</v>
       </c>
       <c r="EW74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>0.55527513574616905</v>
       </c>
       <c r="EX74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>1.2146385664600405</v>
       </c>
       <c r="EY74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>-2.4580639273535416</v>
       </c>
       <c r="EZ74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>0.88740404424991859</v>
       </c>
       <c r="FA74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>0.43071210852643649</v>
       </c>
       <c r="FB74" s="13">
-        <f t="shared" si="88"/>
+        <f t="shared" si="96"/>
         <v>-0.86864431415828691</v>
       </c>
       <c r="FE74" s="17" t="s">
         <v>265</v>
       </c>
       <c r="FF74" s="13">
-        <f t="shared" ref="FF74:FI74" si="89">(FF65*SQRT(44-2))/(SQRT(1-FF65^2))</f>
+        <f t="shared" ref="FF74:FI74" si="97">(FF65*SQRT(44-2))/(SQRT(1-FF65^2))</f>
         <v>0.8454622281254921</v>
       </c>
       <c r="FG74" s="13">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>8.3845640294903948E-2</v>
       </c>
       <c r="FH74" s="13">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>-1.5178842090993305</v>
       </c>
       <c r="FI74" s="13">
-        <f t="shared" si="89"/>
+        <f t="shared" si="97"/>
         <v>0.40878794970494425</v>
       </c>
     </row>
@@ -42275,125 +42538,125 @@
         <v>256</v>
       </c>
       <c r="EC75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-2.5841139284534966</v>
       </c>
       <c r="ED75" s="13" t="e">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>#DIV/0!</v>
       </c>
       <c r="EE75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.70660929775596659</v>
       </c>
       <c r="EF75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.34725168238374349</v>
       </c>
       <c r="EG75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.37500279020971233</v>
       </c>
       <c r="EH75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.84216238218985195</v>
       </c>
       <c r="EI75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-1.5977250990352756</v>
       </c>
       <c r="EJ75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.58492657730826847</v>
       </c>
       <c r="EK75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.87097539644913291</v>
       </c>
       <c r="EL75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.76953929851731262</v>
       </c>
       <c r="EM75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-1.0901740848507484</v>
       </c>
       <c r="EN75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-4.0822627798574684</v>
       </c>
       <c r="EO75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.8931559183071696</v>
       </c>
       <c r="EP75" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.24754166451444329</v>
       </c>
       <c r="EQ75" s="17" t="s">
         <v>256</v>
       </c>
       <c r="ER75" s="13">
-        <f t="shared" ref="ER75:FB75" si="90">(ER66*SQRT(44-2))/(SQRT(1-ER66^2))</f>
+        <f t="shared" ref="ER75:FB75" si="98">(ER66*SQRT(44-2))/(SQRT(1-ER66^2))</f>
         <v>0.25348000523339675</v>
       </c>
       <c r="ES75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>1.0032329498925772</v>
       </c>
       <c r="ET75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>0.85251459077491176</v>
       </c>
       <c r="EU75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>0.47966505710320068</v>
       </c>
       <c r="EV75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>0.83029388249337632</v>
       </c>
       <c r="EW75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>0.91962117523821341</v>
       </c>
       <c r="EX75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>-7.3686847106565048E-2</v>
       </c>
       <c r="EY75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>-1.0781794744828281</v>
       </c>
       <c r="EZ75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>1.9418193640815775</v>
       </c>
       <c r="FA75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>2.783468435822944</v>
       </c>
       <c r="FB75" s="13">
-        <f t="shared" si="90"/>
+        <f t="shared" si="98"/>
         <v>-1.2427037539569505</v>
       </c>
       <c r="FE75" s="17" t="s">
         <v>256</v>
       </c>
       <c r="FF75" s="13">
-        <f t="shared" ref="FF75:FI75" si="91">(FF66*SQRT(44-2))/(SQRT(1-FF66^2))</f>
+        <f t="shared" ref="FF75:FI75" si="99">(FF66*SQRT(44-2))/(SQRT(1-FF66^2))</f>
         <v>-0.13260303858196015</v>
       </c>
       <c r="FG75" s="13">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0.70910395062404674</v>
       </c>
       <c r="FH75" s="13">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>-0.67344552291016302</v>
       </c>
       <c r="FI75" s="13">
-        <f t="shared" si="91"/>
+        <f t="shared" si="99"/>
         <v>0.16225416970585327</v>
       </c>
     </row>
@@ -42475,125 +42738,125 @@
         <v>237</v>
       </c>
       <c r="EC76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.58979006243238397</v>
       </c>
       <c r="ED76" s="13" t="e">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>#DIV/0!</v>
       </c>
       <c r="EE76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.42475873658671226</v>
       </c>
       <c r="EF76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>1.8213879569804228</v>
       </c>
       <c r="EG76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.61143477883440067</v>
       </c>
       <c r="EH76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-1.3686737222855361</v>
       </c>
       <c r="EI76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.31615988633646303</v>
       </c>
       <c r="EJ76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.89081321258213941</v>
       </c>
       <c r="EK76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-1.4170967648154993</v>
       </c>
       <c r="EL76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.67413127302693221</v>
       </c>
       <c r="EM76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>-0.34413739608497329</v>
       </c>
       <c r="EN76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.72694431463931208</v>
       </c>
       <c r="EO76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.983376102501482</v>
       </c>
       <c r="EP76" s="13">
-        <f t="shared" si="83"/>
+        <f t="shared" si="91"/>
         <v>0.68548578486407674</v>
       </c>
       <c r="EQ76" s="17" t="s">
         <v>237</v>
       </c>
       <c r="ER76" s="13">
-        <f t="shared" ref="ER76:FB77" si="92">(ER67*SQRT(44-2))/(SQRT(1-ER67^2))</f>
+        <f t="shared" ref="ER76:FB77" si="100">(ER67*SQRT(44-2))/(SQRT(1-ER67^2))</f>
         <v>0.54679303085063424</v>
       </c>
       <c r="ES76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>-1.3253164602337331</v>
       </c>
       <c r="ET76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0.16010371981489302</v>
       </c>
       <c r="EU76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0.75970967835528136</v>
       </c>
       <c r="EV76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>1.5476814682137729</v>
       </c>
       <c r="EW76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>-0.8156333890157238</v>
       </c>
       <c r="EX76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>-1.1331398849616943</v>
       </c>
       <c r="EY76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>3.7100235962667961E-2</v>
       </c>
       <c r="EZ76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>-0.84845913287546371</v>
       </c>
       <c r="FA76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0.69583777511662759</v>
       </c>
       <c r="FB76" s="13">
-        <f t="shared" si="92"/>
+        <f t="shared" si="100"/>
         <v>0.90269134302990506</v>
       </c>
       <c r="FE76" s="17" t="s">
         <v>237</v>
       </c>
       <c r="FF76" s="13">
-        <f t="shared" ref="FF76:FI76" si="93">(FF67*SQRT(44-2))/(SQRT(1-FF67^2))</f>
+        <f t="shared" ref="FF76:FI76" si="101">(FF67*SQRT(44-2))/(SQRT(1-FF67^2))</f>
         <v>-7.9441754372131121E-2</v>
       </c>
       <c r="FG76" s="13">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>-1.432488218765485</v>
       </c>
       <c r="FH76" s="13">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>-1.9514228509681635E-2</v>
       </c>
       <c r="FI76" s="13">
-        <f t="shared" si="93"/>
+        <f t="shared" si="101"/>
         <v>1.4755334451787769</v>
       </c>
     </row>
@@ -43021,55 +43284,55 @@
         <v>0.10358446157531352</v>
       </c>
       <c r="ED81" s="138">
-        <f t="shared" ref="ED81:EP81" si="94">TDIST(ABS(ED71),42,2)</f>
+        <f t="shared" ref="ED81:EP81" si="102">TDIST(ABS(ED71),42,2)</f>
         <v>1</v>
       </c>
       <c r="EE81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>8.0993834353763519E-2</v>
       </c>
       <c r="EF81" s="162">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>1.5776720944235798E-2</v>
       </c>
       <c r="EG81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>0.29859145718409824</v>
       </c>
       <c r="EH81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>6.2204726444483417E-2</v>
       </c>
       <c r="EI81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>0.24408553789577558</v>
       </c>
       <c r="EJ81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>9.7016134326673407E-3</v>
       </c>
       <c r="EK81" s="162">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>1.2580152276540428E-2</v>
       </c>
       <c r="EL81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>0.41970365396110165</v>
       </c>
       <c r="EM81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>0.79363190650458248</v>
       </c>
       <c r="EN81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>0.92815577446718467</v>
       </c>
       <c r="EO81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>0.20778279765861737</v>
       </c>
       <c r="EP81" s="138">
-        <f t="shared" si="94"/>
+        <f t="shared" si="102"/>
         <v>0.18182655690018187</v>
       </c>
       <c r="EQ81" s="17" t="s">
@@ -43080,43 +43343,43 @@
         <v>0.96466770514968214</v>
       </c>
       <c r="ES81" s="140">
-        <f t="shared" ref="ES81:FB81" si="95">TDIST(ABS(ES71),42,2)</f>
+        <f t="shared" ref="ES81:FB81" si="103">TDIST(ABS(ES71),42,2)</f>
         <v>0.38385551742814339</v>
       </c>
       <c r="ET81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.9217017640768681</v>
       </c>
       <c r="EU81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.52990579318953712</v>
       </c>
       <c r="EV81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.10545027578578485</v>
       </c>
       <c r="EW81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.64564399408051476</v>
       </c>
       <c r="EX81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.53572275618315413</v>
       </c>
       <c r="EY81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.61477621774581848</v>
       </c>
       <c r="EZ81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.46378212829206011</v>
       </c>
       <c r="FA81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.17997080095685175</v>
       </c>
       <c r="FB81" s="140">
-        <f t="shared" si="95"/>
+        <f t="shared" si="103"/>
         <v>0.39765570035495856</v>
       </c>
       <c r="FE81" s="17" t="s">
@@ -43127,15 +43390,15 @@
         <v>0.41506518206703624</v>
       </c>
       <c r="FG81" s="138">
-        <f t="shared" ref="FG81:FI81" si="96">TDIST(ABS(FG71),42,2)</f>
+        <f t="shared" ref="FG81:FI81" si="104">TDIST(ABS(FG71),42,2)</f>
         <v>0.68077539348178395</v>
       </c>
       <c r="FH81" s="138">
-        <f t="shared" si="96"/>
+        <f t="shared" si="104"/>
         <v>0.46779094357637463</v>
       </c>
       <c r="FI81" s="138">
-        <f t="shared" si="96"/>
+        <f t="shared" si="104"/>
         <v>0.52956385931194794</v>
       </c>
     </row>
@@ -43217,125 +43480,125 @@
         <v>275</v>
       </c>
       <c r="EC82" s="138">
-        <f t="shared" ref="EC82:EP86" si="97">TDIST(ABS(EC72),42,2)</f>
+        <f t="shared" ref="EC82:EP86" si="105">TDIST(ABS(EC72),42,2)</f>
         <v>0.41063229592305395</v>
       </c>
       <c r="ED82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>1</v>
       </c>
       <c r="EE82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>2.4658973043165982E-2</v>
       </c>
       <c r="EF82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.39953741651769803</v>
       </c>
       <c r="EG82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.56453029361757112</v>
       </c>
       <c r="EH82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.53443592180807276</v>
       </c>
       <c r="EI82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.24113756038361867</v>
       </c>
       <c r="EJ82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.1433958874344973</v>
       </c>
       <c r="EK82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.70847093944535655</v>
       </c>
       <c r="EL82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.9002553451152332</v>
       </c>
       <c r="EM82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.50503159208780968</v>
       </c>
       <c r="EN82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.4916080146946431</v>
       </c>
       <c r="EO82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>9.7891263200430276E-2</v>
       </c>
       <c r="EP82" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.13230861349992085</v>
       </c>
       <c r="EQ82" s="17" t="s">
         <v>275</v>
       </c>
       <c r="ER82" s="162">
-        <f t="shared" ref="ER82:FB86" si="98">TDIST(ABS(ER72),42,2)</f>
+        <f t="shared" ref="ER82:FB86" si="106">TDIST(ABS(ER72),42,2)</f>
         <v>3.3497556623254952E-2</v>
       </c>
       <c r="ES82" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.89897186166233123</v>
       </c>
       <c r="ET82" s="162">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>2.8609241171502004E-2</v>
       </c>
       <c r="EU82" s="162">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>4.7395606659426846E-2</v>
       </c>
       <c r="EV82" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.19942144471836179</v>
       </c>
       <c r="EW82" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.43573956255741952</v>
       </c>
       <c r="EX82" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.89860234290628649</v>
       </c>
       <c r="EY82" s="156">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>6.835992842896349E-2</v>
       </c>
       <c r="EZ82" s="155">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>1.9295317065964022E-3</v>
       </c>
       <c r="FA82" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.22724747030975143</v>
       </c>
       <c r="FB82" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.2725430286815651</v>
       </c>
       <c r="FE82" s="17" t="s">
         <v>275</v>
       </c>
       <c r="FF82" s="138">
-        <f t="shared" ref="FF82:FI86" si="99">TDIST(ABS(FF72),42,2)</f>
+        <f t="shared" ref="FF82:FI86" si="107">TDIST(ABS(FF72),42,2)</f>
         <v>0.59972820148500161</v>
       </c>
       <c r="FG82" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.47182572339061934</v>
       </c>
       <c r="FH82" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.37315979599437421</v>
       </c>
       <c r="FI82" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.40303420049617544</v>
       </c>
     </row>
@@ -43417,125 +43680,125 @@
         <v>274</v>
       </c>
       <c r="EC83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.19244012973151448</v>
       </c>
       <c r="ED83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>1</v>
       </c>
       <c r="EE83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.46203360462621246</v>
       </c>
       <c r="EF83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.49324578433754829</v>
       </c>
       <c r="EG83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.39709805812032672</v>
       </c>
       <c r="EH83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.54544538465223602</v>
       </c>
       <c r="EI83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.55937368898924578</v>
       </c>
       <c r="EJ83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.63570720705605677</v>
       </c>
       <c r="EK83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.46490112290787533</v>
       </c>
       <c r="EL83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.85921121660055233</v>
       </c>
       <c r="EM83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.87604812818577882</v>
       </c>
       <c r="EN83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>8.7267601357511743E-2</v>
       </c>
       <c r="EO83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.85099698326258211</v>
       </c>
       <c r="EP83" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.83094065167937414</v>
       </c>
       <c r="EQ83" s="17" t="s">
         <v>274</v>
       </c>
       <c r="ER83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.78453817210643795</v>
       </c>
       <c r="ES83" s="162">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>3.2982990204072346E-2</v>
       </c>
       <c r="ET83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.90611703355926798</v>
       </c>
       <c r="EU83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.29327313419483991</v>
       </c>
       <c r="EV83" s="162">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>3.1373652239888757E-2</v>
       </c>
       <c r="EW83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.43758501046383469</v>
       </c>
       <c r="EX83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.96719925050312172</v>
       </c>
       <c r="EY83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.70363613570042371</v>
       </c>
       <c r="EZ83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.44428880693368922</v>
       </c>
       <c r="FA83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.49664146780123908</v>
       </c>
       <c r="FB83" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.95240021368841932</v>
       </c>
       <c r="FE83" s="17" t="s">
         <v>274</v>
       </c>
       <c r="FF83" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.55555376554189717</v>
       </c>
       <c r="FG83" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.30048567118197855</v>
       </c>
       <c r="FH83" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.99235215611965866</v>
       </c>
       <c r="FI83" s="156">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>8.6777990375468433E-2</v>
       </c>
     </row>
@@ -43617,125 +43880,125 @@
         <v>265</v>
       </c>
       <c r="EC84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.64707024527529633</v>
       </c>
       <c r="ED84" s="138" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>#DIV/0!</v>
       </c>
       <c r="EE84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.33269182355514826</v>
       </c>
       <c r="EF84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.66701722890048121</v>
       </c>
       <c r="EG84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.80589545392858564</v>
       </c>
       <c r="EH84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.9549043656502888</v>
       </c>
       <c r="EI84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.49851504028605376</v>
       </c>
       <c r="EJ84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.51107489415503926</v>
       </c>
       <c r="EK84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.56064152409987056</v>
       </c>
       <c r="EL84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.14005271990422413</v>
       </c>
       <c r="EM84" s="155">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>4.2267280638077489E-3</v>
       </c>
       <c r="EN84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.15928376292000423</v>
       </c>
       <c r="EO84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.64665847118504027</v>
       </c>
       <c r="EP84" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.554642842390904</v>
       </c>
       <c r="EQ84" s="17" t="s">
         <v>265</v>
       </c>
       <c r="ER84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.33560490635036855</v>
       </c>
       <c r="ES84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.41359759421513365</v>
       </c>
       <c r="ET84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.64599745921362373</v>
       </c>
       <c r="EU84" s="155">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>8.1828135931208031E-3</v>
       </c>
       <c r="EV84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.23149694422577158</v>
       </c>
       <c r="EW84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.58165215879008214</v>
       </c>
       <c r="EX84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.23128896635015767</v>
       </c>
       <c r="EY84" s="162">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>1.8176330640303461E-2</v>
       </c>
       <c r="EZ84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.3799150812210097</v>
       </c>
       <c r="FA84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.66888011768530808</v>
       </c>
       <c r="FB84" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.38997846883487197</v>
       </c>
       <c r="FE84" s="17" t="s">
         <v>265</v>
       </c>
       <c r="FF84" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.4026437831231805</v>
       </c>
       <c r="FG84" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.93357753166653268</v>
       </c>
       <c r="FH84" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.13653559080469763</v>
       </c>
       <c r="FI84" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.68477227165403765</v>
       </c>
     </row>
@@ -43817,125 +44080,125 @@
         <v>256</v>
       </c>
       <c r="EC85" s="162">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>1.3330689373822277E-2</v>
       </c>
       <c r="ED85" s="138" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>#DIV/0!</v>
       </c>
       <c r="EE85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.48371119870441559</v>
       </c>
       <c r="EF85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.73013635233290419</v>
       </c>
       <c r="EG85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.70954546000819529</v>
       </c>
       <c r="EH85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.40446718064292198</v>
       </c>
       <c r="EI85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.11760151013504011</v>
       </c>
       <c r="EJ85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.56172652679334423</v>
       </c>
       <c r="EK85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.38871893083103271</v>
       </c>
       <c r="EL85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.44587977264731471</v>
       </c>
       <c r="EM85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.2818517760179105</v>
       </c>
       <c r="EN85" s="155">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>1.9550844067722268E-4</v>
       </c>
       <c r="EO85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>6.5240751226129171E-2</v>
       </c>
       <c r="EP85" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.80569522617510148</v>
       </c>
       <c r="EQ85" s="17" t="s">
         <v>256</v>
       </c>
       <c r="ER85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.80113403310686193</v>
       </c>
       <c r="ES85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.3214936704929916</v>
       </c>
       <c r="ET85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.39876400523785038</v>
       </c>
       <c r="EU85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.63395406672393206</v>
       </c>
       <c r="EV85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.41106755840644738</v>
       </c>
       <c r="EW85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.36302253526466721</v>
       </c>
       <c r="EX85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.94160939402140387</v>
       </c>
       <c r="EY85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.28710724217766947</v>
       </c>
       <c r="EZ85" s="156">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>5.8886343483168797E-2</v>
       </c>
       <c r="FA85" s="155">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>8.0270620930543608E-3</v>
       </c>
       <c r="FB85" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.22087048725806144</v>
       </c>
       <c r="FE85" s="17" t="s">
         <v>256</v>
       </c>
       <c r="FF85" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.89514059789966061</v>
       </c>
       <c r="FG85" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.48217788882351087</v>
       </c>
       <c r="FH85" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.50435316086267545</v>
       </c>
       <c r="FI85" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.87188381054341191</v>
       </c>
     </row>
@@ -44017,125 +44280,125 @@
         <v>237</v>
       </c>
       <c r="EC86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.55849119683163473</v>
       </c>
       <c r="ED86" s="138" t="e">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>#DIV/0!</v>
       </c>
       <c r="EE86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.67318074081646861</v>
       </c>
       <c r="EF86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>7.5675717038230353E-2</v>
       </c>
       <c r="EG86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.54420730593769173</v>
       </c>
       <c r="EH86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.17837784963514972</v>
       </c>
       <c r="EI86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.75344708643192215</v>
       </c>
       <c r="EJ86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.37810419143447893</v>
       </c>
       <c r="EK86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.16383031496659581</v>
       </c>
       <c r="EL86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.5039215099771629</v>
       </c>
       <c r="EM86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.73246006992135104</v>
       </c>
       <c r="EN86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.47129268937118629</v>
       </c>
       <c r="EO86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.33105354569984102</v>
       </c>
       <c r="EP86" s="138">
-        <f t="shared" si="97"/>
+        <f t="shared" si="105"/>
         <v>0.49680377308227985</v>
       </c>
       <c r="EQ86" s="17" t="s">
         <v>237</v>
       </c>
       <c r="ER86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.58741446938401676</v>
       </c>
       <c r="ES86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.19223085033950271</v>
       </c>
       <c r="ET86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.87356691372923445</v>
       </c>
       <c r="EU86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.4516715202070487</v>
       </c>
       <c r="EV86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.12920192104267073</v>
       </c>
       <c r="EW86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.41931150297983577</v>
       </c>
       <c r="EX86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.26358271659606375</v>
       </c>
       <c r="EY86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.97058086491208617</v>
       </c>
       <c r="EZ86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.40099221303455623</v>
       </c>
       <c r="FA86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.49036315789572904</v>
       </c>
       <c r="FB86" s="140">
-        <f t="shared" si="98"/>
+        <f t="shared" si="106"/>
         <v>0.37183786377885408</v>
       </c>
       <c r="FE86" s="17" t="s">
         <v>237</v>
       </c>
       <c r="FF86" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.93705857268797454</v>
       </c>
       <c r="FG86" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.15940549874842525</v>
       </c>
       <c r="FH86" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.98452329920845516</v>
       </c>
       <c r="FI86" s="138">
-        <f t="shared" si="99"/>
+        <f t="shared" si="107"/>
         <v>0.1475272313234732</v>
       </c>
     </row>
@@ -44853,6 +45116,9 @@
       <c r="DZ95" s="21"/>
       <c r="EA95" s="42"/>
       <c r="EB95" s="42"/>
+      <c r="EC95" s="13" t="s">
+        <v>443</v>
+      </c>
       <c r="ED95"/>
       <c r="EQ95"/>
     </row>

</xml_diff>

<commit_message>
Adding in charts and graphs
</commit_message>
<xml_diff>
--- a/Masters Project Data.xlsx
+++ b/Masters Project Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="15600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="900" yWindow="0" windowWidth="23260" windowHeight="15600" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1959" uniqueCount="454">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1985" uniqueCount="462">
   <si>
     <t>Timestamp</t>
   </si>
@@ -1386,6 +1386,30 @@
   <si>
     <t>intention vs emotion</t>
   </si>
+  <si>
+    <t>avg</t>
+  </si>
+  <si>
+    <t>stdev</t>
+  </si>
+  <si>
+    <t>emotionality</t>
+  </si>
+  <si>
+    <t>extraversion</t>
+  </si>
+  <si>
+    <t>agreeableness</t>
+  </si>
+  <si>
+    <t>conscientiousness</t>
+  </si>
+  <si>
+    <t>openness to experience</t>
+  </si>
+  <si>
+    <t>Types of Games Played by Players</t>
+  </si>
 </sst>
 </file>
 
@@ -2013,7 +2037,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="194">
+  <cellStyleXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2208,8 +2232,16 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="174">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -2484,6 +2516,9 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2492,8 +2527,26 @@
     <xf numFmtId="0" fontId="4" fillId="6" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="194">
+  <cellStyles count="202">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -2590,6 +2643,10 @@
     <cellStyle name="Followed Hyperlink" xfId="189" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="191" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="193" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="195" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="197" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="199" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="201" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -2686,12 +2743,538 @@
     <cellStyle name="Hyperlink" xfId="188" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="190" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="192" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="194" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="196" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="198" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="200" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="151" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="139"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="39"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Mean Personality Domain Scores (+/-</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> SD)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Analysis'!$AG$62</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Data Analysis'!$AH$63:$BA$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>7.4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.6</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Data Analysis'!$AH$63:$BA$63</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="6"/>
+                  <c:pt idx="0">
+                    <c:v>7.4</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.6</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>9.7</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.5</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>5.5</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>7.5</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Analysis'!$AH$61:$BA$61</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Honesty/Humility</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Emotionality</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Extraversion</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Agreeableness</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Conscientiousness</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Openness to Experience</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Analysis'!$AH$62:$BA$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0" formatCode="0.0">
+                  <c:v>32.7</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29.6</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>32.2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.3</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>35.8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="2139703000"/>
+        <c:axId val="2139711992"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2139703000"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2139711992"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2139711992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="50.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2139703000"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="139"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="39"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr b="1" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" b="1" i="0">
+                <a:latin typeface="Helvetica Neue Medium"/>
+              </a:rPr>
+              <a:t>Types of Games Played by Players (+/- SE)</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="1"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Data Analysis'!$EC$103:$ED$103</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Types of Games Played by Players</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Data Analysis'!$EE$102:$EP$102</c:f>
+              <c:strCache>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>Role-playing</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Puzzle</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Simulation</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>First-person Shooter</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Third-person shooter</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Adventure</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Strategy</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Sports</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Fighting</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>Survival</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>Arcade</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>Driving</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Data Analysis'!$EE$103:$EP$103</c:f>
+              <c:numCache>
+                <c:formatCode>0%</c:formatCode>
+                <c:ptCount val="12"/>
+                <c:pt idx="0">
+                  <c:v>0.795454545454545</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.590909090909091</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.363636363636364</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.590909090909091</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.431818181818182</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.659090909090909</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.545454545454545</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.113636363636364</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.386363636363636</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.318181818181818</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.522727272727273</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.295454545454545</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2084967720"/>
+        <c:axId val="2139885688"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2084967720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="2139885688"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2139885688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2084967720"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:latin typeface="Helvetica Neue Light"/>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>44450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>38</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>88</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>135</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>91</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>143</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>115</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -13342,8 +13925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FK135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="FL21" sqref="FL21"/>
+    <sheetView tabSelected="1" topLeftCell="CL91" workbookViewId="0">
+      <selection activeCell="DU101" sqref="DU101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0"/>
@@ -15375,10 +15958,7 @@
       <c r="B6" s="8">
         <v>2</v>
       </c>
-      <c r="E6" s="8">
-        <f>'Form Responses 1'!C4</f>
-        <v>0</v>
-      </c>
+      <c r="E6" s="8"/>
       <c r="F6" s="8"/>
       <c r="G6" s="3" t="s">
         <v>423</v>
@@ -23382,7 +23962,7 @@
       <c r="FI20" s="3">
         <v>3</v>
       </c>
-      <c r="FK20" s="171" t="s">
+      <c r="FK20" s="172" t="s">
         <v>452</v>
       </c>
     </row>
@@ -23918,7 +24498,7 @@
       <c r="FI21" s="3">
         <v>1</v>
       </c>
-      <c r="FK21" s="172">
+      <c r="FK21" s="173">
         <f>TTEST(FG4:FG47,FI4:FI47,2,1)</f>
         <v>1.82772962096142E-3</v>
       </c>
@@ -24454,7 +25034,7 @@
       <c r="FI22" s="3">
         <v>2</v>
       </c>
-      <c r="FK22" s="172"/>
+      <c r="FK22" s="173"/>
     </row>
     <row r="23" spans="1:167" ht="15.75" customHeight="1">
       <c r="A23" s="7"/>
@@ -24987,7 +25567,7 @@
       <c r="FI23" s="3">
         <v>2</v>
       </c>
-      <c r="FK23" s="172" t="s">
+      <c r="FK23" s="173" t="s">
         <v>453</v>
       </c>
     </row>
@@ -25522,7 +26102,7 @@
       <c r="FI24" s="3">
         <v>4</v>
       </c>
-      <c r="FK24" s="173">
+      <c r="FK24" s="174">
         <f>TTEST(FH4:FH47,FI4:FI47,2,1)</f>
         <v>3.9848349682986814E-4</v>
       </c>
@@ -37237,10 +37817,7 @@
       </c>
       <c r="C47" s="23"/>
       <c r="D47" s="23"/>
-      <c r="E47" s="8">
-        <f>'Form Responses 1'!C45</f>
-        <v>0</v>
-      </c>
+      <c r="E47" s="8"/>
       <c r="F47" s="8"/>
       <c r="G47" s="3" t="s">
         <v>427</v>
@@ -37770,6 +38347,10 @@
       <c r="A48" s="7"/>
       <c r="C48" s="7"/>
       <c r="D48" s="7"/>
+      <c r="E48" s="9">
+        <f>_xlfn.STDEV.S(E4:E46)</f>
+        <v>5.9122503188508997</v>
+      </c>
       <c r="G48" s="3" t="s">
         <v>434</v>
       </c>
@@ -37886,6 +38467,10 @@
       <c r="DU49" s="13"/>
       <c r="EA49" s="13"/>
       <c r="EB49" s="66"/>
+      <c r="EC49" s="6">
+        <f>35/44</f>
+        <v>0.79545454545454541</v>
+      </c>
       <c r="EE49" s="6" t="s">
         <v>409</v>
       </c>
@@ -37926,7 +38511,7 @@
       <c r="D50" s="147"/>
       <c r="E50" s="65">
         <f>AVERAGE(E4:E47)</f>
-        <v>28.5</v>
+        <v>29.857142857142858</v>
       </c>
       <c r="F50" s="86" t="s">
         <v>422</v>
@@ -37957,29 +38542,43 @@
       <c r="AH50" s="67"/>
       <c r="AM50" s="11"/>
       <c r="AQ50" s="11"/>
-      <c r="AU50" s="11"/>
+      <c r="AU50" s="11" t="s">
+        <v>456</v>
+      </c>
       <c r="AZ50" s="11"/>
       <c r="BA50" s="66"/>
       <c r="BG50" s="11"/>
       <c r="BL50" s="13"/>
-      <c r="BO50" s="13"/>
+      <c r="BO50" s="13" t="s">
+        <v>457</v>
+      </c>
       <c r="BS50" s="13"/>
       <c r="BT50" s="67"/>
       <c r="BW50" s="13"/>
       <c r="CB50" s="13"/>
-      <c r="CH50" s="13"/>
+      <c r="CH50" s="13" t="s">
+        <v>458</v>
+      </c>
       <c r="CL50" s="13"/>
       <c r="CM50" s="66"/>
       <c r="CQ50" s="11"/>
       <c r="CU50" s="13"/>
-      <c r="CZ50" s="13"/>
+      <c r="CZ50" s="13" t="s">
+        <v>459</v>
+      </c>
       <c r="DG50" s="13"/>
       <c r="DH50" s="67"/>
       <c r="DL50" s="13"/>
       <c r="DP50" s="13"/>
-      <c r="DU50" s="13"/>
+      <c r="DU50" s="13" t="s">
+        <v>460</v>
+      </c>
       <c r="EA50" s="13"/>
       <c r="EB50" s="66"/>
+      <c r="EC50" s="6">
+        <f>COUNTIF(EC$4:EC$47,1)</f>
+        <v>3</v>
+      </c>
       <c r="ER50" s="6" t="s">
         <v>361</v>
       </c>
@@ -38028,7 +38627,7 @@
       <c r="D51" s="142"/>
       <c r="E51" s="76">
         <f>MEDIAN(E4:E47)</f>
-        <v>28.5</v>
+        <v>29</v>
       </c>
       <c r="F51" s="11" t="s">
         <v>424</v>
@@ -38077,6 +38676,10 @@
       <c r="DU51" s="13"/>
       <c r="EA51" s="13"/>
       <c r="EB51" s="66"/>
+      <c r="EC51" s="6">
+        <f>COUNTIF(EC$4:EC$47,2)</f>
+        <v>2</v>
+      </c>
       <c r="EE51" s="6">
         <f>COUNTIF(EE4:EE47,1)</f>
         <v>35</v>
@@ -38261,6 +38864,10 @@
       <c r="DW52" s="21"/>
       <c r="DY52" s="30"/>
       <c r="DZ52" s="21"/>
+      <c r="EC52" s="6">
+        <f>COUNTIF(EC$4:EC$47,3)</f>
+        <v>0</v>
+      </c>
       <c r="ED52"/>
       <c r="EE52" s="13">
         <f>COUNTIF(EE4:EE47,0)</f>
@@ -38852,6 +39459,10 @@
       <c r="EB53" s="139">
         <f t="shared" si="68"/>
         <v>35.795454545454547</v>
+      </c>
+      <c r="EC53" s="6">
+        <f>COUNTIF(EC$4:EC$47,4)</f>
+        <v>2</v>
       </c>
       <c r="ED53"/>
       <c r="EE53" s="151">
@@ -39034,6 +39645,10 @@
       <c r="DW54" s="21"/>
       <c r="DY54" s="30"/>
       <c r="DZ54" s="21"/>
+      <c r="EC54" s="6">
+        <f>COUNTIF(EC$4:EC$47,5)</f>
+        <v>2</v>
+      </c>
       <c r="ED54"/>
       <c r="EQ54"/>
       <c r="FC54" s="45" t="s">
@@ -39198,6 +39813,10 @@
       </c>
       <c r="EB55" s="13">
         <v>50</v>
+      </c>
+      <c r="EC55" s="6">
+        <f>COUNTIF(EC$4:EC$47,6)</f>
+        <v>15</v>
       </c>
       <c r="ED55"/>
       <c r="EQ55"/>
@@ -39272,6 +39891,10 @@
       <c r="DW56" s="21"/>
       <c r="DY56" s="30"/>
       <c r="DZ56" s="21"/>
+      <c r="EC56" s="6">
+        <f>COUNTIF(EC$4:EC$47,7)</f>
+        <v>20</v>
+      </c>
       <c r="ED56" s="6"/>
       <c r="EQ56" s="6"/>
       <c r="FC56" s="144"/>
@@ -39834,19 +40457,19 @@
       <c r="FE58" s="13" t="s">
         <v>444</v>
       </c>
-      <c r="FF58" s="170">
+      <c r="FF58" s="171">
         <f>(FF51+FF52)/(FF51+FF52+FF53+FF54)</f>
         <v>0.45454545454545453</v>
       </c>
-      <c r="FG58" s="170">
+      <c r="FG58" s="171">
         <f t="shared" ref="FG58:FI58" si="75">(FG51+FG52)/(FG51+FG52+FG53+FG54)</f>
         <v>0.68181818181818177</v>
       </c>
-      <c r="FH58" s="170">
+      <c r="FH58" s="171">
         <f t="shared" si="75"/>
         <v>0.59090909090909094</v>
       </c>
-      <c r="FI58" s="170">
+      <c r="FI58" s="171">
         <f t="shared" si="75"/>
         <v>0.27272727272727271</v>
       </c>
@@ -39946,19 +40569,19 @@
       <c r="FE59" s="13" t="s">
         <v>445</v>
       </c>
-      <c r="FF59" s="170">
+      <c r="FF59" s="171">
         <f>(FF53+FF54)/(FF51+FF52+FF53+FF54)</f>
         <v>0.54545454545454541</v>
       </c>
-      <c r="FG59" s="170">
+      <c r="FG59" s="171">
         <f t="shared" ref="FG59:FI59" si="76">(FG53+FG54)/(FG51+FG52+FG53+FG54)</f>
         <v>0.31818181818181818</v>
       </c>
-      <c r="FH59" s="170">
+      <c r="FH59" s="171">
         <f t="shared" si="76"/>
         <v>0.40909090909090912</v>
       </c>
-      <c r="FI59" s="170">
+      <c r="FI59" s="171">
         <f t="shared" si="76"/>
         <v>0.72727272727272729</v>
       </c>
@@ -40085,20 +40708,44 @@
       <c r="AE61" s="21"/>
       <c r="AF61" s="71"/>
       <c r="AG61" s="38"/>
-      <c r="AH61" s="38"/>
-      <c r="AK61" s="30"/>
-      <c r="AM61" s="41"/>
-      <c r="AO61" s="30"/>
-      <c r="AP61" s="21"/>
-      <c r="AQ61" s="41"/>
-      <c r="AS61" s="30"/>
-      <c r="AU61" s="41"/>
-      <c r="AX61" s="30"/>
-      <c r="AZ61" s="41"/>
-      <c r="BA61" s="77"/>
-      <c r="BC61" s="30"/>
-      <c r="BE61" s="30"/>
-      <c r="BG61" s="41"/>
+      <c r="AH61" s="175" t="s">
+        <v>237</v>
+      </c>
+      <c r="AI61" s="175"/>
+      <c r="AJ61" s="175"/>
+      <c r="AK61" s="175"/>
+      <c r="AL61" s="176"/>
+      <c r="AM61" s="177" t="s">
+        <v>256</v>
+      </c>
+      <c r="AN61" s="168"/>
+      <c r="AO61" s="178"/>
+      <c r="AP61" s="179"/>
+      <c r="AQ61" s="177" t="s">
+        <v>265</v>
+      </c>
+      <c r="AR61" s="168"/>
+      <c r="AS61" s="178"/>
+      <c r="AT61" s="168"/>
+      <c r="AU61" s="177" t="s">
+        <v>274</v>
+      </c>
+      <c r="AV61" s="168"/>
+      <c r="AW61" s="168"/>
+      <c r="AX61" s="178"/>
+      <c r="AY61" s="168"/>
+      <c r="AZ61" s="177" t="s">
+        <v>275</v>
+      </c>
+      <c r="BA61" s="180" t="s">
+        <v>294</v>
+      </c>
+      <c r="BB61" s="168"/>
+      <c r="BC61" s="178"/>
+      <c r="BD61" s="168"/>
+      <c r="BE61" s="178"/>
+      <c r="BF61" s="168"/>
+      <c r="BG61" s="177"/>
       <c r="BH61" s="30"/>
       <c r="BL61" s="42"/>
       <c r="BO61" s="42"/>
@@ -40242,18 +40889,32 @@
       <c r="AD62" s="79"/>
       <c r="AE62" s="80"/>
       <c r="AF62" s="81"/>
-      <c r="AG62" s="38"/>
-      <c r="AH62" s="38"/>
+      <c r="AG62" s="38" t="s">
+        <v>454</v>
+      </c>
+      <c r="AH62" s="139">
+        <v>32.700000000000003</v>
+      </c>
       <c r="AK62" s="79"/>
-      <c r="AM62" s="36"/>
+      <c r="AM62" s="36">
+        <v>29.6</v>
+      </c>
       <c r="AO62" s="79"/>
       <c r="AP62" s="80"/>
-      <c r="AQ62" s="36"/>
+      <c r="AQ62" s="36">
+        <v>31</v>
+      </c>
       <c r="AS62" s="79"/>
-      <c r="AU62" s="36"/>
+      <c r="AU62" s="36">
+        <v>32.200000000000003</v>
+      </c>
       <c r="AX62" s="79"/>
-      <c r="AZ62" s="36"/>
-      <c r="BA62" s="78"/>
+      <c r="AZ62" s="36">
+        <v>37.299999999999997</v>
+      </c>
+      <c r="BA62" s="78">
+        <v>35.799999999999997</v>
+      </c>
       <c r="BC62" s="79"/>
       <c r="BE62" s="79"/>
       <c r="BG62" s="36"/>
@@ -40435,18 +41096,32 @@
       <c r="AD63" s="79"/>
       <c r="AE63" s="80"/>
       <c r="AF63" s="81"/>
-      <c r="AG63" s="38"/>
-      <c r="AH63" s="38"/>
+      <c r="AG63" s="38" t="s">
+        <v>455</v>
+      </c>
+      <c r="AH63" s="38">
+        <v>7.4</v>
+      </c>
       <c r="AK63" s="79"/>
-      <c r="AM63" s="36"/>
+      <c r="AM63" s="36">
+        <v>5.6</v>
+      </c>
       <c r="AO63" s="79"/>
       <c r="AP63" s="80"/>
-      <c r="AQ63" s="36"/>
+      <c r="AQ63" s="36">
+        <v>9.6999999999999993</v>
+      </c>
       <c r="AS63" s="79"/>
-      <c r="AU63" s="36"/>
+      <c r="AU63" s="36">
+        <v>7.5</v>
+      </c>
       <c r="AX63" s="79"/>
-      <c r="AZ63" s="36"/>
-      <c r="BA63" s="78"/>
+      <c r="AZ63" s="36">
+        <v>5.5</v>
+      </c>
+      <c r="BA63" s="78">
+        <v>7.5</v>
+      </c>
       <c r="BC63" s="79"/>
       <c r="BE63" s="79"/>
       <c r="BG63" s="36"/>
@@ -40919,7 +41594,7 @@
         <f>CORREL(BT4:BT47,EL4:EL47)</f>
         <v>-0.22607104599635461</v>
       </c>
-      <c r="EM65" s="169">
+      <c r="EM65" s="170">
         <f>CORREL(BT4:BT47,EM4:EM47)</f>
         <v>-0.42299982697678978</v>
       </c>
@@ -44640,7 +45315,7 @@
       <c r="EI89" s="167" t="s">
         <v>442</v>
       </c>
-      <c r="EJ89" s="168" t="s">
+      <c r="EJ89" s="169" t="s">
         <v>440</v>
       </c>
       <c r="EQ89"/>
@@ -44723,7 +45398,7 @@
       <c r="ED90"/>
       <c r="EH90" s="166"/>
       <c r="EI90" s="167"/>
-      <c r="EJ90" s="168"/>
+      <c r="EJ90" s="169"/>
       <c r="EQ90"/>
     </row>
     <row r="91" spans="2:165" s="13" customFormat="1" ht="15.75" customHeight="1">
@@ -44804,7 +45479,7 @@
       <c r="ED91"/>
       <c r="EH91" s="166"/>
       <c r="EI91" s="167"/>
-      <c r="EJ91" s="168"/>
+      <c r="EJ91" s="169"/>
       <c r="EQ91"/>
     </row>
     <row r="92" spans="2:165" s="13" customFormat="1" ht="15.75" customHeight="1">
@@ -45666,6 +46341,42 @@
       <c r="EA102" s="42"/>
       <c r="EB102" s="42"/>
       <c r="ED102"/>
+      <c r="EE102" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="EF102" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="EG102" s="6" t="s">
+        <v>338</v>
+      </c>
+      <c r="EH102" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="EI102" s="6" t="s">
+        <v>339</v>
+      </c>
+      <c r="EJ102" s="6" t="s">
+        <v>340</v>
+      </c>
+      <c r="EK102" s="6" t="s">
+        <v>341</v>
+      </c>
+      <c r="EL102" s="6" t="s">
+        <v>342</v>
+      </c>
+      <c r="EM102" s="6" t="s">
+        <v>343</v>
+      </c>
+      <c r="EN102" s="6" t="s">
+        <v>344</v>
+      </c>
+      <c r="EO102" s="6" t="s">
+        <v>345</v>
+      </c>
+      <c r="EP102" s="6" t="s">
+        <v>346</v>
+      </c>
       <c r="EQ102"/>
     </row>
     <row r="103" spans="2:147" s="13" customFormat="1" ht="15.75" customHeight="1">
@@ -45743,7 +46454,46 @@
       <c r="DZ103" s="21"/>
       <c r="EA103" s="42"/>
       <c r="EB103" s="42"/>
+      <c r="EC103" s="13" t="s">
+        <v>461</v>
+      </c>
       <c r="ED103"/>
+      <c r="EE103" s="171">
+        <v>0.79545454545454541</v>
+      </c>
+      <c r="EF103" s="171">
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="EG103" s="171">
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="EH103" s="171">
+        <v>0.59090909090909094</v>
+      </c>
+      <c r="EI103" s="171">
+        <v>0.43181818181818182</v>
+      </c>
+      <c r="EJ103" s="171">
+        <v>0.65909090909090906</v>
+      </c>
+      <c r="EK103" s="171">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="EL103" s="171">
+        <v>0.11363636363636363</v>
+      </c>
+      <c r="EM103" s="171">
+        <v>0.38636363636363635</v>
+      </c>
+      <c r="EN103" s="171">
+        <v>0.31818181818181818</v>
+      </c>
+      <c r="EO103" s="171">
+        <v>0.52272727272727271</v>
+      </c>
+      <c r="EP103" s="171">
+        <v>0.29545454545454547</v>
+      </c>
       <c r="EQ103"/>
     </row>
     <row r="104" spans="2:147" s="13" customFormat="1" ht="15.75" customHeight="1">
@@ -48244,10 +48994,11 @@
       <c r="FD135" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="53">
+  <mergeCells count="54">
     <mergeCell ref="EH89:EH91"/>
     <mergeCell ref="EI89:EI91"/>
     <mergeCell ref="EJ89:EJ91"/>
+    <mergeCell ref="AH61:AL61"/>
     <mergeCell ref="FD1:FD3"/>
     <mergeCell ref="EE69:EN70"/>
     <mergeCell ref="EC59:EN60"/>
@@ -48301,6 +49052,7 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>